<commit_message>
Updated JSON Schema and examples as per C. Aniekwe's recommendations. Bumped Data Dictionary version to draft v1.3
</commit_message>
<xml_diff>
--- a/files_and_resources/Data Dictionary.xlsx
+++ b/files_and_resources/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubarak Abdu-Aguye\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA90586-3044-4AD0-9F61-AE7464960749}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386018C8-BDE8-47AF-BA29-8C286A8A7E88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="238">
   <si>
     <t>ID</t>
   </si>
@@ -268,9 +268,6 @@
     <t>Viral Load/EID Result Request</t>
   </si>
   <si>
-    <t>facilityID</t>
-  </si>
-  <si>
     <t>The unique identifier for the facility requesting the result</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
     <t>The unique identifier of the facility that is now receiving the result. Used for result validation.</t>
   </si>
   <si>
-    <t>sendingPCRLab</t>
-  </si>
-  <si>
     <t>The identifier (e.g LIMS ID) of the PCR lab sending/returning the results</t>
   </si>
   <si>
@@ -722,6 +716,36 @@
   </si>
   <si>
     <t>Improper Packaging</t>
+  </si>
+  <si>
+    <t>Name of the facility requesting the result</t>
+  </si>
+  <si>
+    <t>receivingPCRLabId</t>
+  </si>
+  <si>
+    <t>The unique identifier for the PCR lab doing the analysis</t>
+  </si>
+  <si>
+    <t>receivingPCRLabName</t>
+  </si>
+  <si>
+    <t>Name of the PCR lab doing the analysis</t>
+  </si>
+  <si>
+    <t>receivingFacilityName</t>
+  </si>
+  <si>
+    <t>The name of the facility that is now receiving the result</t>
+  </si>
+  <si>
+    <t>sendingPCRLabID</t>
+  </si>
+  <si>
+    <t>sendingPCRLabName</t>
+  </si>
+  <si>
+    <t>The name of the PCR lab sending/returning the results</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7068A318-C14F-4D04-B583-D7B1DF373F65}">
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView topLeftCell="C70" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,7 +1486,7 @@
         <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1699,7 +1723,7 @@
         <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -1719,7 +1743,7 @@
         <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -1739,7 +1763,7 @@
         <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
@@ -1759,7 +1783,7 @@
         <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D29" t="s">
         <v>18</v>
@@ -1779,7 +1803,7 @@
         <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
@@ -1799,7 +1823,7 @@
         <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
@@ -1819,7 +1843,7 @@
         <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
         <v>23</v>
@@ -1842,7 +1866,7 @@
         <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
         <v>46</v>
@@ -1862,7 +1886,7 @@
         <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
         <v>29</v>
@@ -1882,7 +1906,7 @@
         <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D35" t="s">
         <v>31</v>
@@ -1902,7 +1926,7 @@
         <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D36" t="s">
         <v>43</v>
@@ -1917,7 +1941,7 @@
         <v>13</v>
       </c>
       <c r="H36" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
@@ -1925,13 +1949,13 @@
         <v>74</v>
       </c>
       <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" t="s">
         <v>114</v>
-      </c>
-      <c r="D37" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" t="s">
-        <v>116</v>
       </c>
       <c r="F37" t="s">
         <v>42</v>
@@ -1945,7 +1969,7 @@
         <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
         <v>33</v>
@@ -1968,13 +1992,13 @@
         <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D39" t="s">
         <v>67</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F39" t="s">
         <v>45</v>
@@ -1988,7 +2012,7 @@
         <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
         <v>69</v>
@@ -2008,13 +2032,13 @@
         <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D41" t="s">
         <v>75</v>
       </c>
       <c r="E41" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F41" t="s">
         <v>42</v>
@@ -2031,22 +2055,22 @@
         <v>74</v>
       </c>
       <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" t="s">
         <v>119</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F42" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
         <v>120</v>
-      </c>
-      <c r="E42" t="s">
-        <v>121</v>
-      </c>
-      <c r="F42" t="s">
-        <v>111</v>
-      </c>
-      <c r="G42" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -2054,13 +2078,13 @@
         <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F43" t="s">
         <v>45</v>
@@ -2069,7 +2093,7 @@
         <v>57</v>
       </c>
       <c r="H43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
@@ -2077,13 +2101,13 @@
         <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D44" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
@@ -2092,10 +2116,10 @@
         <v>57</v>
       </c>
       <c r="H44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I44" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
@@ -2103,13 +2127,13 @@
         <v>74</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F45" t="s">
         <v>42</v>
@@ -2118,7 +2142,7 @@
         <v>13</v>
       </c>
       <c r="I45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
@@ -2126,13 +2150,13 @@
         <v>74</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D46" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E46" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F46" t="s">
         <v>42</v>
@@ -2141,7 +2165,7 @@
         <v>13</v>
       </c>
       <c r="I46" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
@@ -2149,22 +2173,22 @@
         <v>74</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D47" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" t="s">
         <v>190</v>
-      </c>
-      <c r="E47" t="s">
-        <v>191</v>
-      </c>
-      <c r="F47" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
@@ -2172,13 +2196,13 @@
         <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E48" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F48" t="s">
         <v>12</v>
@@ -2187,7 +2211,7 @@
         <v>13</v>
       </c>
       <c r="I48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
@@ -2195,13 +2219,13 @@
         <v>74</v>
       </c>
       <c r="C49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E49" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F49" t="s">
         <v>42</v>
@@ -2210,7 +2234,7 @@
         <v>13</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
@@ -2218,22 +2242,22 @@
         <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D50" t="s">
+        <v>198</v>
+      </c>
+      <c r="E50" t="s">
+        <v>199</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" t="s">
         <v>200</v>
-      </c>
-      <c r="E50" t="s">
-        <v>201</v>
-      </c>
-      <c r="F50" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2241,10 +2265,10 @@
         <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G51" t="s">
         <v>57</v>
@@ -2255,10 +2279,10 @@
         <v>74</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D52" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G52" t="s">
         <v>57</v>
@@ -2269,10 +2293,10 @@
         <v>74</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D53" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G53" t="s">
         <v>57</v>
@@ -2283,10 +2307,10 @@
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D54" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G54" t="s">
         <v>57</v>
@@ -2297,7 +2321,7 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D55" t="s">
         <v>61</v>
@@ -2317,7 +2341,7 @@
         <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D56" t="s">
         <v>63</v>
@@ -2337,7 +2361,7 @@
         <v>74</v>
       </c>
       <c r="C57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D57" t="s">
         <v>65</v>
@@ -2357,7 +2381,7 @@
         <v>74</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D58" t="s">
         <v>72</v>
@@ -2377,10 +2401,10 @@
         <v>77</v>
       </c>
       <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" t="s">
         <v>78</v>
-      </c>
-      <c r="E59" t="s">
-        <v>79</v>
       </c>
       <c r="F59" t="s">
         <v>12</v>
@@ -2394,19 +2418,19 @@
         <v>77</v>
       </c>
       <c r="D60" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="E60" t="s">
+        <v>228</v>
+      </c>
+      <c r="F60" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" t="s">
+        <v>13</v>
+      </c>
+      <c r="I60" t="s">
         <v>81</v>
-      </c>
-      <c r="F60" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" t="s">
-        <v>13</v>
-      </c>
-      <c r="I60" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
@@ -2414,61 +2438,70 @@
         <v>77</v>
       </c>
       <c r="D61" t="s">
-        <v>20</v>
+        <v>229</v>
       </c>
       <c r="E61" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="F61" t="s">
         <v>12</v>
       </c>
       <c r="G61" t="s">
         <v>13</v>
+      </c>
+      <c r="I61" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>215</v>
+        <v>77</v>
       </c>
       <c r="D62" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
       <c r="E62" t="s">
-        <v>84</v>
+        <v>232</v>
       </c>
       <c r="F62" t="s">
         <v>12</v>
       </c>
       <c r="G62" t="s">
         <v>13</v>
+      </c>
+      <c r="I62" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>215</v>
+        <v>77</v>
       </c>
       <c r="D63" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E63" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F63" t="s">
         <v>12</v>
       </c>
       <c r="G63" t="s">
         <v>13</v>
+      </c>
+      <c r="I63" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>215</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="E64" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F64" t="s">
         <v>12</v>
@@ -2479,59 +2512,47 @@
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F65" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G65" t="s">
         <v>13</v>
-      </c>
-      <c r="I65" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>215</v>
-      </c>
-      <c r="C66" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="E66" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="F66" t="s">
         <v>12</v>
       </c>
       <c r="G66" t="s">
         <v>13</v>
-      </c>
-      <c r="I66" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>215</v>
-      </c>
-      <c r="C67" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D67" t="s">
-        <v>26</v>
+        <v>233</v>
       </c>
       <c r="E67" t="s">
-        <v>27</v>
+        <v>234</v>
       </c>
       <c r="F67" t="s">
         <v>12</v>
@@ -2542,16 +2563,13 @@
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>215</v>
-      </c>
-      <c r="C68" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D68" t="s">
-        <v>46</v>
+        <v>235</v>
       </c>
       <c r="E68" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
@@ -2562,76 +2580,79 @@
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>215</v>
-      </c>
-      <c r="C69" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D69" t="s">
-        <v>91</v>
+        <v>236</v>
       </c>
       <c r="E69" t="s">
-        <v>92</v>
+        <v>237</v>
       </c>
       <c r="F69" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G69" t="s">
         <v>13</v>
+      </c>
+      <c r="I69" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>215</v>
-      </c>
-      <c r="C70" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D70" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E70" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F70" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G70" t="s">
         <v>13</v>
+      </c>
+      <c r="I70" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C71" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D71" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="E71" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="F71" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G71" t="s">
         <v>13</v>
+      </c>
+      <c r="I71" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C72" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D72" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="E72" t="s">
-        <v>213</v>
+        <v>27</v>
       </c>
       <c r="F72" t="s">
         <v>12</v>
@@ -2642,19 +2663,19 @@
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
+        <v>213</v>
+      </c>
+      <c r="C73" t="s">
         <v>215</v>
       </c>
-      <c r="C73" t="s">
-        <v>217</v>
-      </c>
       <c r="D73" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="E73" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="F73" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G73" t="s">
         <v>13</v>
@@ -2662,19 +2683,19 @@
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
+        <v>213</v>
+      </c>
+      <c r="C74" t="s">
         <v>215</v>
       </c>
-      <c r="C74" t="s">
-        <v>217</v>
-      </c>
       <c r="D74" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="E74" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="F74" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G74" t="s">
         <v>13</v>
@@ -2682,39 +2703,42 @@
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
+        <v>213</v>
+      </c>
+      <c r="C75" t="s">
         <v>215</v>
       </c>
-      <c r="C75" t="s">
-        <v>217</v>
-      </c>
       <c r="D75" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="E75" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="F75" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G75" t="s">
         <v>13</v>
+      </c>
+      <c r="I75" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
+        <v>213</v>
+      </c>
+      <c r="C76" t="s">
         <v>215</v>
       </c>
-      <c r="C76" t="s">
-        <v>217</v>
-      </c>
       <c r="D76" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
       <c r="E76" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
       <c r="F76" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G76" t="s">
         <v>13</v>
@@ -2722,42 +2746,39 @@
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" t="s">
         <v>215</v>
       </c>
-      <c r="C77" t="s">
-        <v>217</v>
-      </c>
       <c r="D77" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="E77" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="F77" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G77" t="s">
         <v>13</v>
-      </c>
-      <c r="I77" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
+        <v>213</v>
+      </c>
+      <c r="C78" t="s">
         <v>215</v>
       </c>
-      <c r="C78" t="s">
-        <v>217</v>
-      </c>
       <c r="D78" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="E78" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="F78" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="G78" t="s">
         <v>13</v>
@@ -2765,16 +2786,19 @@
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="C79" t="s">
+        <v>215</v>
       </c>
       <c r="D79" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="E79" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G79" t="s">
         <v>13</v>
@@ -2782,16 +2806,19 @@
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="C80" t="s">
+        <v>215</v>
       </c>
       <c r="D80" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E80" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F80" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G80" t="s">
         <v>13</v>
@@ -2799,13 +2826,16 @@
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="C81" t="s">
+        <v>215</v>
       </c>
       <c r="D81" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E81" t="s">
-        <v>88</v>
+        <v>211</v>
       </c>
       <c r="F81" t="s">
         <v>12</v>
@@ -2816,62 +2846,59 @@
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="C82" t="s">
+        <v>215</v>
       </c>
       <c r="D82" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="E82" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="F82" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G82" t="s">
         <v>13</v>
-      </c>
-      <c r="I82" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C83" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D83" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E83" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="F83" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G83" t="s">
         <v>13</v>
-      </c>
-      <c r="I83" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C84" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D84" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="E84" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="F84" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G84" t="s">
         <v>13</v>
@@ -2879,19 +2906,19 @@
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C85" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D85" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="E85" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G85" t="s">
         <v>13</v>
@@ -2899,39 +2926,42 @@
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C86" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D86" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E86" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="F86" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G86" t="s">
         <v>13</v>
+      </c>
+      <c r="I86" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C87" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D87" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="E87" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F87" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="G87" t="s">
         <v>13</v>
@@ -2939,19 +2969,16 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>218</v>
-      </c>
-      <c r="C88" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D88" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="E88" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F88" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G88" t="s">
         <v>13</v>
@@ -2959,42 +2986,33 @@
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>218</v>
-      </c>
-      <c r="C89" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D89" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E89" t="s">
-        <v>213</v>
+        <v>85</v>
       </c>
       <c r="F89" t="s">
         <v>12</v>
       </c>
       <c r="G89" t="s">
         <v>13</v>
-      </c>
-      <c r="I89" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>218</v>
-      </c>
-      <c r="C90" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D90" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="E90" t="s">
-        <v>99</v>
+        <v>234</v>
       </c>
       <c r="F90" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G90" t="s">
         <v>13</v>
@@ -3002,19 +3020,16 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>218</v>
-      </c>
-      <c r="C91" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D91" t="s">
-        <v>100</v>
+        <v>235</v>
       </c>
       <c r="E91" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="F91" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G91" t="s">
         <v>13</v>
@@ -3022,19 +3037,16 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>218</v>
-      </c>
-      <c r="C92" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D92" t="s">
-        <v>102</v>
+        <v>236</v>
       </c>
       <c r="E92" t="s">
-        <v>103</v>
+        <v>237</v>
       </c>
       <c r="F92" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G92" t="s">
         <v>13</v>
@@ -3042,62 +3054,62 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>218</v>
-      </c>
-      <c r="C93" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D93" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E93" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="F93" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G93" t="s">
         <v>13</v>
+      </c>
+      <c r="I93" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C94" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D94" t="s">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="E94" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="F94" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G94" t="s">
         <v>13</v>
       </c>
       <c r="I94" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C95" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D95" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="E95" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="F95" t="s">
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="G95" t="s">
         <v>13</v>
@@ -3105,25 +3117,334 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" t="s">
         <v>218</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
+        <v>29</v>
+      </c>
+      <c r="E96" t="s">
+        <v>30</v>
+      </c>
+      <c r="F96" t="s">
+        <v>12</v>
+      </c>
+      <c r="G96" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>216</v>
+      </c>
+      <c r="C97" t="s">
+        <v>218</v>
+      </c>
+      <c r="D97" t="s">
+        <v>31</v>
+      </c>
+      <c r="E97" t="s">
+        <v>32</v>
+      </c>
+      <c r="F97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>216</v>
+      </c>
+      <c r="C98" t="s">
+        <v>218</v>
+      </c>
+      <c r="D98" t="s">
+        <v>33</v>
+      </c>
+      <c r="E98" t="s">
+        <v>34</v>
+      </c>
+      <c r="F98" t="s">
+        <v>12</v>
+      </c>
+      <c r="G98" t="s">
+        <v>13</v>
+      </c>
+      <c r="I98" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>216</v>
+      </c>
+      <c r="C99" t="s">
+        <v>218</v>
+      </c>
+      <c r="D99" t="s">
+        <v>43</v>
+      </c>
+      <c r="E99" t="s">
+        <v>44</v>
+      </c>
+      <c r="F99" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>216</v>
+      </c>
+      <c r="C100" t="s">
+        <v>218</v>
+      </c>
+      <c r="D100" t="s">
+        <v>46</v>
+      </c>
+      <c r="E100" t="s">
+        <v>88</v>
+      </c>
+      <c r="F100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>216</v>
+      </c>
+      <c r="C101" t="s">
+        <v>218</v>
+      </c>
+      <c r="D101" t="s">
+        <v>89</v>
+      </c>
+      <c r="E101" t="s">
+        <v>90</v>
+      </c>
+      <c r="F101" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>216</v>
+      </c>
+      <c r="C102" t="s">
+        <v>218</v>
+      </c>
+      <c r="D102" t="s">
+        <v>91</v>
+      </c>
+      <c r="E102" t="s">
+        <v>92</v>
+      </c>
+      <c r="F102" t="s">
+        <v>45</v>
+      </c>
+      <c r="G102" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>216</v>
+      </c>
+      <c r="C103" t="s">
+        <v>218</v>
+      </c>
+      <c r="D103" t="s">
+        <v>93</v>
+      </c>
+      <c r="E103" t="s">
+        <v>94</v>
+      </c>
+      <c r="F103" t="s">
+        <v>45</v>
+      </c>
+      <c r="G103" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>216</v>
+      </c>
+      <c r="C104" t="s">
+        <v>218</v>
+      </c>
+      <c r="D104" t="s">
+        <v>95</v>
+      </c>
+      <c r="E104" t="s">
+        <v>211</v>
+      </c>
+      <c r="F104" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" t="s">
+        <v>13</v>
+      </c>
+      <c r="I104" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>216</v>
+      </c>
+      <c r="C105" t="s">
+        <v>218</v>
+      </c>
+      <c r="D105" t="s">
+        <v>96</v>
+      </c>
+      <c r="E105" t="s">
+        <v>97</v>
+      </c>
+      <c r="F105" t="s">
+        <v>45</v>
+      </c>
+      <c r="G105" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>216</v>
+      </c>
+      <c r="C106" t="s">
+        <v>218</v>
+      </c>
+      <c r="D106" t="s">
+        <v>98</v>
+      </c>
+      <c r="E106" t="s">
+        <v>99</v>
+      </c>
+      <c r="F106" t="s">
+        <v>45</v>
+      </c>
+      <c r="G106" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>216</v>
+      </c>
+      <c r="C107" t="s">
+        <v>218</v>
+      </c>
+      <c r="D107" t="s">
+        <v>100</v>
+      </c>
+      <c r="E107" t="s">
+        <v>101</v>
+      </c>
+      <c r="F107" t="s">
+        <v>45</v>
+      </c>
+      <c r="G107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>216</v>
+      </c>
+      <c r="C108" t="s">
+        <v>218</v>
+      </c>
+      <c r="D108" t="s">
+        <v>102</v>
+      </c>
+      <c r="E108" t="s">
+        <v>103</v>
+      </c>
+      <c r="F108" t="s">
+        <v>45</v>
+      </c>
+      <c r="G108" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>216</v>
+      </c>
+      <c r="C109" t="s">
+        <v>218</v>
+      </c>
+      <c r="D109" t="s">
+        <v>104</v>
+      </c>
+      <c r="E109" t="s">
+        <v>105</v>
+      </c>
+      <c r="F109" t="s">
+        <v>42</v>
+      </c>
+      <c r="G109" t="s">
+        <v>13</v>
+      </c>
+      <c r="I109" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>216</v>
+      </c>
+      <c r="C110" t="s">
+        <v>218</v>
+      </c>
+      <c r="D110" t="s">
+        <v>107</v>
+      </c>
+      <c r="E110" t="s">
+        <v>108</v>
+      </c>
+      <c r="F110" t="s">
+        <v>109</v>
+      </c>
+      <c r="G110" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>216</v>
+      </c>
+      <c r="C111" t="s">
+        <v>218</v>
+      </c>
+      <c r="D111" t="s">
         <v>220</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E111" t="s">
+        <v>221</v>
+      </c>
+      <c r="F111" t="s">
+        <v>109</v>
+      </c>
+      <c r="G111" t="s">
+        <v>57</v>
+      </c>
+      <c r="I111" t="s">
         <v>222</v>
-      </c>
-      <c r="E96" t="s">
-        <v>223</v>
-      </c>
-      <c r="F96" t="s">
-        <v>111</v>
-      </c>
-      <c r="G96" t="s">
-        <v>57</v>
-      </c>
-      <c r="I96" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3136,7 +3457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97107629-23FF-4FFF-81A6-C8B1543F2D0F}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="C57" sqref="C57:C61"/>
     </sheetView>
   </sheetViews>
@@ -3153,13 +3474,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3167,10 +3488,10 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3178,10 +3499,10 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3189,10 +3510,10 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3200,10 +3521,10 @@
         <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3211,10 +3532,10 @@
         <v>35</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3222,10 +3543,10 @@
         <v>35</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3233,10 +3554,10 @@
         <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3247,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3258,7 +3579,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3269,7 +3590,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -3280,7 +3601,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -3288,10 +3609,10 @@
         <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3299,10 +3620,10 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -3313,7 +3634,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -3324,7 +3645,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -3335,7 +3656,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -3346,7 +3667,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -3357,7 +3678,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -3368,7 +3689,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -3379,7 +3700,7 @@
         <v>7</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -3390,7 +3711,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -3401,7 +3722,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -3412,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -3423,403 +3744,403 @@
         <v>4</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>171</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C31" s="5">
         <v>2</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C32" s="5">
         <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C34" s="5">
         <v>5</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C35" s="5">
         <v>6</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C36" s="5">
         <v>7</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C37" s="5">
         <v>8</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C38" s="5">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C39" s="5">
         <v>2</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C40" s="5">
         <v>3</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C41" s="5">
         <v>4</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
+        <v>190</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
+        <v>200</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="D47" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" s="5">
         <v>1</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49" s="5">
         <v>2</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C50" s="5">
         <v>1</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C51" s="5">
         <v>2</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C52" s="5">
         <v>3</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C53" s="5">
         <v>4</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C57" s="5">
         <v>1</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C58" s="5">
         <v>2</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C59" s="5">
         <v>3</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C60" s="5">
         <v>4</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C61" s="5">
         <v>5</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Data Dictionary to Draft Version 1.4 with updated drug regimen concepts
</commit_message>
<xml_diff>
--- a/files_and_resources/Data Dictionary.xlsx
+++ b/files_and_resources/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubarak Abdu-Aguye\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386018C8-BDE8-47AF-BA29-8C286A8A7E88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB224EB2-96D5-48C2-A2BF-BEE64F6AEF67}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="415">
   <si>
     <t>ID</t>
   </si>
@@ -214,9 +214,6 @@
     <t>The drug regimen the patient is on.</t>
   </si>
   <si>
-    <t>DRUG_REGIMEN</t>
-  </si>
-  <si>
     <t>sampleOrderedBy</t>
   </si>
   <si>
@@ -746,6 +743,540 @@
   </si>
   <si>
     <t>The name of the PCR lab sending/returning the results</t>
+  </si>
+  <si>
+    <t>ARV_REGIMEN</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>1e</t>
+  </si>
+  <si>
+    <t>1f</t>
+  </si>
+  <si>
+    <t>1g</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>1n</t>
+  </si>
+  <si>
+    <t>1o</t>
+  </si>
+  <si>
+    <t>1p</t>
+  </si>
+  <si>
+    <t>1q</t>
+  </si>
+  <si>
+    <t>1r</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>1t</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>1v</t>
+  </si>
+  <si>
+    <t>1w</t>
+  </si>
+  <si>
+    <t>1x</t>
+  </si>
+  <si>
+    <t>1y</t>
+  </si>
+  <si>
+    <t>1z</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>2c</t>
+  </si>
+  <si>
+    <t>2d</t>
+  </si>
+  <si>
+    <t>2e</t>
+  </si>
+  <si>
+    <t>2f</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>2i</t>
+  </si>
+  <si>
+    <t>2j</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>2m</t>
+  </si>
+  <si>
+    <t>2n</t>
+  </si>
+  <si>
+    <t>2o</t>
+  </si>
+  <si>
+    <t>2p</t>
+  </si>
+  <si>
+    <t>2q</t>
+  </si>
+  <si>
+    <t>2r</t>
+  </si>
+  <si>
+    <t>2s</t>
+  </si>
+  <si>
+    <t>2t</t>
+  </si>
+  <si>
+    <t>2u</t>
+  </si>
+  <si>
+    <t>2v</t>
+  </si>
+  <si>
+    <t>2w</t>
+  </si>
+  <si>
+    <t>2x</t>
+  </si>
+  <si>
+    <t>2y</t>
+  </si>
+  <si>
+    <t>2g</t>
+  </si>
+  <si>
+    <t>4b</t>
+  </si>
+  <si>
+    <t>4c</t>
+  </si>
+  <si>
+    <t>4d</t>
+  </si>
+  <si>
+    <t>4f</t>
+  </si>
+  <si>
+    <t>4g</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>5b</t>
+  </si>
+  <si>
+    <t>5c</t>
+  </si>
+  <si>
+    <t>5d</t>
+  </si>
+  <si>
+    <t>5f</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t>6c</t>
+  </si>
+  <si>
+    <t>6d</t>
+  </si>
+  <si>
+    <t>6e</t>
+  </si>
+  <si>
+    <t>6f</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>3e</t>
+  </si>
+  <si>
+    <t>3f</t>
+  </si>
+  <si>
+    <t>3g</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>3i</t>
+  </si>
+  <si>
+    <t>3j</t>
+  </si>
+  <si>
+    <t>3k</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>3n</t>
+  </si>
+  <si>
+    <t>3o</t>
+  </si>
+  <si>
+    <t>3p</t>
+  </si>
+  <si>
+    <t>3q</t>
+  </si>
+  <si>
+    <t>3r</t>
+  </si>
+  <si>
+    <t>3s</t>
+  </si>
+  <si>
+    <t>3t</t>
+  </si>
+  <si>
+    <t>3u</t>
+  </si>
+  <si>
+    <t>3v</t>
+  </si>
+  <si>
+    <t>3w</t>
+  </si>
+  <si>
+    <t>3x</t>
+  </si>
+  <si>
+    <t>AZT-3TC-EFV</t>
+  </si>
+  <si>
+    <t>AZT-3TC-NVP</t>
+  </si>
+  <si>
+    <t>TDF-FTC-EFV</t>
+  </si>
+  <si>
+    <t>TDF-FTC-NVP</t>
+  </si>
+  <si>
+    <t>TDF-3TC-EFV</t>
+  </si>
+  <si>
+    <t>TDF-3TC-NVP</t>
+  </si>
+  <si>
+    <t>ABC-3TC-AZT</t>
+  </si>
+  <si>
+    <t>TDF-3TC-AZT</t>
+  </si>
+  <si>
+    <t>TDF-3TC-DTG</t>
+  </si>
+  <si>
+    <t>TDF-FTC-DTG</t>
+  </si>
+  <si>
+    <t>ABC-3TC-DTG</t>
+  </si>
+  <si>
+    <t>ABC-FTC-DTG</t>
+  </si>
+  <si>
+    <t>D4T-3TC-EFV</t>
+  </si>
+  <si>
+    <t>ABC-FTC-EFV</t>
+  </si>
+  <si>
+    <t>ABC-FTC-NVP</t>
+  </si>
+  <si>
+    <t>ABC-3TC-TDF</t>
+  </si>
+  <si>
+    <t>D4T-3TC-ABC</t>
+  </si>
+  <si>
+    <t>AZT-TDF-NVP</t>
+  </si>
+  <si>
+    <t>DDI-3TC-EFV</t>
+  </si>
+  <si>
+    <t>ABC-3TC-DDI</t>
+  </si>
+  <si>
+    <t>AZT-3TC-DTG</t>
+  </si>
+  <si>
+    <t>Adult First Line Others</t>
+  </si>
+  <si>
+    <t>TDF-FTC-LPV/r</t>
+  </si>
+  <si>
+    <t>TDF-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>TDF-FTC-ATV/r</t>
+  </si>
+  <si>
+    <t>TDF-3TC-ATV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-ATV/r</t>
+  </si>
+  <si>
+    <t>ABC-AZT-LPV/r</t>
+  </si>
+  <si>
+    <t>DDI-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>ABC-DDI-LPV/r</t>
+  </si>
+  <si>
+    <t>AZT-TDF-ATV/r</t>
+  </si>
+  <si>
+    <t>ABC-3TC-ATV/r</t>
+  </si>
+  <si>
+    <t>ABC-DDI-SQV/r</t>
+  </si>
+  <si>
+    <t>TDF-FTC-SQV/r</t>
+  </si>
+  <si>
+    <t>TDF-3TC-SQV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-SQV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-IDV/r</t>
+  </si>
+  <si>
+    <t>D4T-3TC-IDV/r</t>
+  </si>
+  <si>
+    <t>TDF-FTC-IDV/r</t>
+  </si>
+  <si>
+    <t>TDF-3TC-IDV/r</t>
+  </si>
+  <si>
+    <t>TDF-DDI-IDV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-DRV/r</t>
+  </si>
+  <si>
+    <t>TDF-3TC-DRV/r</t>
+  </si>
+  <si>
+    <t>Adult Second Line Others</t>
+  </si>
+  <si>
+    <t>ABC-3TC-EFV</t>
+  </si>
+  <si>
+    <t>ABC-3TC-NVP</t>
+  </si>
+  <si>
+    <t>d4T-3TC-NVP</t>
+  </si>
+  <si>
+    <t>Child First Line Others</t>
+  </si>
+  <si>
+    <t>ABC-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>d4T-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>ddi-3TC-NVP</t>
+  </si>
+  <si>
+    <t>Child Second Line Others</t>
+  </si>
+  <si>
+    <t>DRV/r + 2 NRTIs + 2 NNRTI</t>
+  </si>
+  <si>
+    <t>DRV/r +2NRTIs</t>
+  </si>
+  <si>
+    <t>DRV/r-DTG + 1-2 NRTIs</t>
+  </si>
+  <si>
+    <t>DRV/r+RAL + 1-2NRTIs</t>
+  </si>
+  <si>
+    <t>DTG+2 NRTIs</t>
+  </si>
+  <si>
+    <t>RAL(or DTG) + 2 NRTIs</t>
+  </si>
+  <si>
+    <t>AZT-TDF-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>AZT-TDF-FTC-LPV/r</t>
+  </si>
+  <si>
+    <t>TDF-AZT-3TC-ATV/r</t>
+  </si>
+  <si>
+    <t>TDF-3TC-DTG-LPV/r</t>
+  </si>
+  <si>
+    <t>TDF-FTC-AZT-ATV/r</t>
+  </si>
+  <si>
+    <t>TDF-3TC-DTG-DRV-RTV</t>
+  </si>
+  <si>
+    <t>ABC-3TC-DTG-ATV/r</t>
+  </si>
+  <si>
+    <t>ABC-3TC-DTG-DRV-RTV</t>
+  </si>
+  <si>
+    <t>ABC-3TC-AZT-LPV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-LPV-SQV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-LPV-ATV/r</t>
+  </si>
+  <si>
+    <t>ABC-3TC-AZT-EFV</t>
+  </si>
+  <si>
+    <t>ABC-3TC-AZT-ATV/r</t>
+  </si>
+  <si>
+    <t>TDF-FTC-LPV-ATV/r</t>
+  </si>
+  <si>
+    <t>TDF-AZT-FTC-IDV/r</t>
+  </si>
+  <si>
+    <t>TDF-AZT-FTC-SQV/r</t>
+  </si>
+  <si>
+    <t>TDF-AZT-3TC-IDV/r</t>
+  </si>
+  <si>
+    <t>TDF-AZT-3TC-SQV/r</t>
+  </si>
+  <si>
+    <t>AZT-3TC-RAL</t>
+  </si>
+  <si>
+    <t>ABC-3TC-RAL</t>
+  </si>
+  <si>
+    <t>TDF-3TC-RAL</t>
+  </si>
+  <si>
+    <t>AZT-RAL-ATV/r</t>
+  </si>
+  <si>
+    <t>DDI-3TC-IND/r</t>
+  </si>
+  <si>
+    <t>ABC-3TC-LPV-ATV/r</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adult 1st line ARV regimen </t>
+  </si>
+  <si>
+    <t>Adult 2nd line ARV regimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adult 1st line ARV regimen/ Child 1st line ARV regimen</t>
+  </si>
+  <si>
+    <t>Child 1st line ARV regimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Child 2nd line ARV regimen</t>
+  </si>
+  <si>
+    <t>Child 3rd Line ARV Regimens</t>
+  </si>
+  <si>
+    <t>Adult 3rd Line ARV Regimens</t>
   </si>
 </sst>
 </file>
@@ -834,7 +1365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -852,6 +1383,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7068A318-C14F-4D04-B583-D7B1DF373F65}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+    <sheetView topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1486,7 +2020,7 @@
         <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1595,7 +2129,7 @@
         <v>57</v>
       </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
@@ -1606,10 +2140,10 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
         <v>61</v>
-      </c>
-      <c r="E20" t="s">
-        <v>62</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -1626,10 +2160,10 @@
         <v>28</v>
       </c>
       <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
         <v>63</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
       </c>
       <c r="F21" t="s">
         <v>45</v>
@@ -1646,10 +2180,10 @@
         <v>28</v>
       </c>
       <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
         <v>65</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
@@ -1666,10 +2200,10 @@
         <v>28</v>
       </c>
       <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
         <v>67</v>
-      </c>
-      <c r="E23" t="s">
-        <v>68</v>
       </c>
       <c r="F23" t="s">
         <v>45</v>
@@ -1686,13 +2220,13 @@
         <v>28</v>
       </c>
       <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
         <v>69</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>70</v>
-      </c>
-      <c r="F24" t="s">
-        <v>71</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>
@@ -1706,10 +2240,10 @@
         <v>28</v>
       </c>
       <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
         <v>72</v>
-      </c>
-      <c r="E25" t="s">
-        <v>73</v>
       </c>
       <c r="F25" t="s">
         <v>45</v>
@@ -1720,10 +2254,10 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -1740,10 +2274,10 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
@@ -1760,10 +2294,10 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
@@ -1780,10 +2314,10 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" t="s">
         <v>18</v>
@@ -1800,10 +2334,10 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
@@ -1820,10 +2354,10 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
@@ -1840,10 +2374,10 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
         <v>23</v>
@@ -1863,10 +2397,10 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
         <v>46</v>
@@ -1883,10 +2417,10 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D34" t="s">
         <v>29</v>
@@ -1903,10 +2437,10 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D35" t="s">
         <v>31</v>
@@ -1923,10 +2457,10 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
         <v>43</v>
@@ -1941,21 +2475,21 @@
         <v>13</v>
       </c>
       <c r="H36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" t="s">
         <v>112</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>113</v>
-      </c>
-      <c r="E37" t="s">
-        <v>114</v>
       </c>
       <c r="F37" t="s">
         <v>42</v>
@@ -1966,10 +2500,10 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D38" t="s">
         <v>33</v>
@@ -1989,16 +2523,16 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F39" t="s">
         <v>45</v>
@@ -2009,19 +2543,19 @@
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" t="s">
         <v>69</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>70</v>
-      </c>
-      <c r="F40" t="s">
-        <v>71</v>
       </c>
       <c r="G40" t="s">
         <v>13</v>
@@ -2029,16 +2563,16 @@
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" t="s">
         <v>74</v>
       </c>
-      <c r="C41" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" t="s">
-        <v>75</v>
-      </c>
       <c r="E41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F41" t="s">
         <v>42</v>
@@ -2047,44 +2581,44 @@
         <v>13</v>
       </c>
       <c r="I41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" t="s">
         <v>117</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>118</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
+        <v>108</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
         <v>119</v>
-      </c>
-      <c r="F42" t="s">
-        <v>109</v>
-      </c>
-      <c r="G42" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
         <v>121</v>
-      </c>
-      <c r="E43" t="s">
-        <v>122</v>
       </c>
       <c r="F43" t="s">
         <v>45</v>
@@ -2093,21 +2627,21 @@
         <v>57</v>
       </c>
       <c r="H43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44" t="s">
         <v>124</v>
-      </c>
-      <c r="E44" t="s">
-        <v>125</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
@@ -2116,24 +2650,24 @@
         <v>57</v>
       </c>
       <c r="H44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" t="s">
         <v>174</v>
-      </c>
-      <c r="E45" t="s">
-        <v>175</v>
       </c>
       <c r="F45" t="s">
         <v>42</v>
@@ -2142,21 +2676,21 @@
         <v>13</v>
       </c>
       <c r="I45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" t="s">
+        <v>183</v>
+      </c>
+      <c r="E46" t="s">
         <v>184</v>
-      </c>
-      <c r="E46" t="s">
-        <v>185</v>
       </c>
       <c r="F46" t="s">
         <v>42</v>
@@ -2165,45 +2699,45 @@
         <v>13</v>
       </c>
       <c r="I46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D47" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" t="s">
         <v>188</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" t="s">
         <v>189</v>
-      </c>
-      <c r="F47" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D48" t="s">
+        <v>192</v>
+      </c>
+      <c r="E48" t="s">
         <v>193</v>
       </c>
-      <c r="E48" t="s">
-        <v>194</v>
-      </c>
       <c r="F48" t="s">
         <v>12</v>
       </c>
@@ -2211,21 +2745,21 @@
         <v>13</v>
       </c>
       <c r="I48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D49" t="s">
+        <v>194</v>
+      </c>
+      <c r="E49" t="s">
         <v>195</v>
-      </c>
-      <c r="E49" t="s">
-        <v>196</v>
       </c>
       <c r="F49" t="s">
         <v>42</v>
@@ -2234,41 +2768,41 @@
         <v>13</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D50" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" t="s">
         <v>198</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" t="s">
         <v>199</v>
-      </c>
-      <c r="F50" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G51" t="s">
         <v>57</v>
@@ -2276,13 +2810,13 @@
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G52" t="s">
         <v>57</v>
@@ -2290,13 +2824,13 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G53" t="s">
         <v>57</v>
@@ -2304,13 +2838,13 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G54" t="s">
         <v>57</v>
@@ -2318,16 +2852,16 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D55" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" t="s">
         <v>61</v>
-      </c>
-      <c r="E55" t="s">
-        <v>62</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
@@ -2338,16 +2872,16 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D56" t="s">
+        <v>62</v>
+      </c>
+      <c r="E56" t="s">
         <v>63</v>
-      </c>
-      <c r="E56" t="s">
-        <v>64</v>
       </c>
       <c r="F56" t="s">
         <v>45</v>
@@ -2358,16 +2892,16 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" t="s">
         <v>65</v>
-      </c>
-      <c r="E57" t="s">
-        <v>66</v>
       </c>
       <c r="F57" t="s">
         <v>12</v>
@@ -2378,16 +2912,16 @@
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D58" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" t="s">
         <v>72</v>
-      </c>
-      <c r="E58" t="s">
-        <v>73</v>
       </c>
       <c r="F58" t="s">
         <v>45</v>
@@ -2398,13 +2932,13 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D59" t="s">
         <v>10</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F59" t="s">
         <v>12</v>
@@ -2415,13 +2949,13 @@
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D60" t="s">
         <v>14</v>
       </c>
       <c r="E60" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F60" t="s">
         <v>12</v>
@@ -2430,19 +2964,19 @@
         <v>13</v>
       </c>
       <c r="I60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D61" t="s">
+        <v>228</v>
+      </c>
+      <c r="E61" t="s">
         <v>229</v>
       </c>
-      <c r="E61" t="s">
-        <v>230</v>
-      </c>
       <c r="F61" t="s">
         <v>12</v>
       </c>
@@ -2450,19 +2984,19 @@
         <v>13</v>
       </c>
       <c r="I61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D62" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" t="s">
         <v>231</v>
       </c>
-      <c r="E62" t="s">
-        <v>232</v>
-      </c>
       <c r="F62" t="s">
         <v>12</v>
       </c>
@@ -2470,38 +3004,38 @@
         <v>13</v>
       </c>
       <c r="I62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D63" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" t="s">
         <v>79</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" t="s">
         <v>80</v>
-      </c>
-      <c r="F63" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D64" t="s">
         <v>20</v>
       </c>
       <c r="E64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F64" t="s">
         <v>12</v>
@@ -2512,13 +3046,13 @@
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D65" t="s">
         <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
@@ -2529,13 +3063,13 @@
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D66" t="s">
+        <v>83</v>
+      </c>
+      <c r="E66" t="s">
         <v>84</v>
-      </c>
-      <c r="E66" t="s">
-        <v>85</v>
       </c>
       <c r="F66" t="s">
         <v>12</v>
@@ -2546,13 +3080,13 @@
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D67" t="s">
+        <v>232</v>
+      </c>
+      <c r="E67" t="s">
         <v>233</v>
-      </c>
-      <c r="E67" t="s">
-        <v>234</v>
       </c>
       <c r="F67" t="s">
         <v>12</v>
@@ -2563,13 +3097,13 @@
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
@@ -2580,13 +3114,13 @@
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D69" t="s">
+        <v>235</v>
+      </c>
+      <c r="E69" t="s">
         <v>236</v>
-      </c>
-      <c r="E69" t="s">
-        <v>237</v>
       </c>
       <c r="F69" t="s">
         <v>42</v>
@@ -2595,18 +3129,18 @@
         <v>13</v>
       </c>
       <c r="I69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F70" t="s">
         <v>42</v>
@@ -2615,15 +3149,15 @@
         <v>13</v>
       </c>
       <c r="I70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
+        <v>212</v>
+      </c>
+      <c r="C71" t="s">
         <v>213</v>
-      </c>
-      <c r="C71" t="s">
-        <v>214</v>
       </c>
       <c r="D71" t="s">
         <v>23</v>
@@ -2643,10 +3177,10 @@
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
+        <v>212</v>
+      </c>
+      <c r="C72" t="s">
         <v>213</v>
-      </c>
-      <c r="C72" t="s">
-        <v>214</v>
       </c>
       <c r="D72" t="s">
         <v>26</v>
@@ -2663,10 +3197,10 @@
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D73" t="s">
         <v>29</v>
@@ -2683,10 +3217,10 @@
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C74" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D74" t="s">
         <v>31</v>
@@ -2703,10 +3237,10 @@
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C75" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
         <v>33</v>
@@ -2726,10 +3260,10 @@
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D76" t="s">
         <v>43</v>
@@ -2746,16 +3280,16 @@
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D77" t="s">
         <v>46</v>
       </c>
       <c r="E77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F77" t="s">
         <v>12</v>
@@ -2766,16 +3300,16 @@
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C78" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D78" t="s">
+        <v>88</v>
+      </c>
+      <c r="E78" t="s">
         <v>89</v>
-      </c>
-      <c r="E78" t="s">
-        <v>90</v>
       </c>
       <c r="F78" t="s">
         <v>12</v>
@@ -2786,16 +3320,16 @@
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D79" t="s">
+        <v>90</v>
+      </c>
+      <c r="E79" t="s">
         <v>91</v>
-      </c>
-      <c r="E79" t="s">
-        <v>92</v>
       </c>
       <c r="F79" t="s">
         <v>45</v>
@@ -2806,16 +3340,16 @@
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D80" t="s">
+        <v>92</v>
+      </c>
+      <c r="E80" t="s">
         <v>93</v>
-      </c>
-      <c r="E80" t="s">
-        <v>94</v>
       </c>
       <c r="F80" t="s">
         <v>45</v>
@@ -2826,16 +3360,16 @@
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F81" t="s">
         <v>12</v>
@@ -2846,16 +3380,16 @@
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D82" t="s">
+        <v>95</v>
+      </c>
+      <c r="E82" t="s">
         <v>96</v>
-      </c>
-      <c r="E82" t="s">
-        <v>97</v>
       </c>
       <c r="F82" t="s">
         <v>45</v>
@@ -2866,16 +3400,16 @@
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D83" t="s">
+        <v>97</v>
+      </c>
+      <c r="E83" t="s">
         <v>98</v>
-      </c>
-      <c r="E83" t="s">
-        <v>99</v>
       </c>
       <c r="F83" t="s">
         <v>45</v>
@@ -2886,16 +3420,16 @@
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C84" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D84" t="s">
+        <v>99</v>
+      </c>
+      <c r="E84" t="s">
         <v>100</v>
-      </c>
-      <c r="E84" t="s">
-        <v>101</v>
       </c>
       <c r="F84" t="s">
         <v>45</v>
@@ -2906,16 +3440,16 @@
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C85" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D85" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" t="s">
         <v>102</v>
-      </c>
-      <c r="E85" t="s">
-        <v>103</v>
       </c>
       <c r="F85" t="s">
         <v>45</v>
@@ -2926,16 +3460,16 @@
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C86" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E86" t="s">
         <v>104</v>
-      </c>
-      <c r="E86" t="s">
-        <v>105</v>
       </c>
       <c r="F86" t="s">
         <v>42</v>
@@ -2944,24 +3478,24 @@
         <v>13</v>
       </c>
       <c r="I86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D87" t="s">
+        <v>106</v>
+      </c>
+      <c r="E87" t="s">
         <v>107</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>108</v>
-      </c>
-      <c r="F87" t="s">
-        <v>109</v>
       </c>
       <c r="G87" t="s">
         <v>13</v>
@@ -2969,13 +3503,13 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D88" t="s">
         <v>20</v>
       </c>
       <c r="E88" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
@@ -2986,13 +3520,13 @@
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D89" t="s">
+        <v>83</v>
+      </c>
+      <c r="E89" t="s">
         <v>84</v>
-      </c>
-      <c r="E89" t="s">
-        <v>85</v>
       </c>
       <c r="F89" t="s">
         <v>12</v>
@@ -3003,13 +3537,13 @@
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D90" t="s">
+        <v>232</v>
+      </c>
+      <c r="E90" t="s">
         <v>233</v>
-      </c>
-      <c r="E90" t="s">
-        <v>234</v>
       </c>
       <c r="F90" t="s">
         <v>12</v>
@@ -3020,13 +3554,13 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D91" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E91" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F91" t="s">
         <v>12</v>
@@ -3037,13 +3571,13 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D92" t="s">
+        <v>235</v>
+      </c>
+      <c r="E92" t="s">
         <v>236</v>
-      </c>
-      <c r="E92" t="s">
-        <v>237</v>
       </c>
       <c r="F92" t="s">
         <v>12</v>
@@ -3054,13 +3588,13 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E93" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F93" t="s">
         <v>42</v>
@@ -3069,15 +3603,15 @@
         <v>13</v>
       </c>
       <c r="I93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
+        <v>215</v>
+      </c>
+      <c r="C94" t="s">
         <v>216</v>
-      </c>
-      <c r="C94" t="s">
-        <v>217</v>
       </c>
       <c r="D94" t="s">
         <v>23</v>
@@ -3097,10 +3631,10 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
+        <v>215</v>
+      </c>
+      <c r="C95" t="s">
         <v>216</v>
-      </c>
-      <c r="C95" t="s">
-        <v>217</v>
       </c>
       <c r="D95" t="s">
         <v>26</v>
@@ -3117,10 +3651,10 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C96" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D96" t="s">
         <v>29</v>
@@ -3137,10 +3671,10 @@
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C97" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D97" t="s">
         <v>31</v>
@@ -3157,10 +3691,10 @@
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C98" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D98" t="s">
         <v>33</v>
@@ -3180,10 +3714,10 @@
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C99" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D99" t="s">
         <v>43</v>
@@ -3200,16 +3734,16 @@
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C100" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D100" t="s">
         <v>46</v>
       </c>
       <c r="E100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F100" t="s">
         <v>12</v>
@@ -3220,16 +3754,16 @@
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D101" t="s">
+        <v>88</v>
+      </c>
+      <c r="E101" t="s">
         <v>89</v>
-      </c>
-      <c r="E101" t="s">
-        <v>90</v>
       </c>
       <c r="F101" t="s">
         <v>12</v>
@@ -3240,16 +3774,16 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C102" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D102" t="s">
+        <v>90</v>
+      </c>
+      <c r="E102" t="s">
         <v>91</v>
-      </c>
-      <c r="E102" t="s">
-        <v>92</v>
       </c>
       <c r="F102" t="s">
         <v>45</v>
@@ -3260,16 +3794,16 @@
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C103" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D103" t="s">
+        <v>92</v>
+      </c>
+      <c r="E103" t="s">
         <v>93</v>
-      </c>
-      <c r="E103" t="s">
-        <v>94</v>
       </c>
       <c r="F103" t="s">
         <v>45</v>
@@ -3280,39 +3814,39 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C104" t="s">
+        <v>217</v>
+      </c>
+      <c r="D104" t="s">
+        <v>94</v>
+      </c>
+      <c r="E104" t="s">
+        <v>210</v>
+      </c>
+      <c r="F104" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" t="s">
+        <v>13</v>
+      </c>
+      <c r="I104" t="s">
         <v>218</v>
-      </c>
-      <c r="D104" t="s">
-        <v>95</v>
-      </c>
-      <c r="E104" t="s">
-        <v>211</v>
-      </c>
-      <c r="F104" t="s">
-        <v>12</v>
-      </c>
-      <c r="G104" t="s">
-        <v>13</v>
-      </c>
-      <c r="I104" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C105" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D105" t="s">
+        <v>95</v>
+      </c>
+      <c r="E105" t="s">
         <v>96</v>
-      </c>
-      <c r="E105" t="s">
-        <v>97</v>
       </c>
       <c r="F105" t="s">
         <v>45</v>
@@ -3323,16 +3857,16 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C106" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D106" t="s">
+        <v>97</v>
+      </c>
+      <c r="E106" t="s">
         <v>98</v>
-      </c>
-      <c r="E106" t="s">
-        <v>99</v>
       </c>
       <c r="F106" t="s">
         <v>45</v>
@@ -3343,16 +3877,16 @@
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D107" t="s">
+        <v>99</v>
+      </c>
+      <c r="E107" t="s">
         <v>100</v>
-      </c>
-      <c r="E107" t="s">
-        <v>101</v>
       </c>
       <c r="F107" t="s">
         <v>45</v>
@@ -3363,16 +3897,16 @@
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C108" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D108" t="s">
+        <v>101</v>
+      </c>
+      <c r="E108" t="s">
         <v>102</v>
-      </c>
-      <c r="E108" t="s">
-        <v>103</v>
       </c>
       <c r="F108" t="s">
         <v>45</v>
@@ -3383,16 +3917,16 @@
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C109" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D109" t="s">
+        <v>103</v>
+      </c>
+      <c r="E109" t="s">
         <v>104</v>
-      </c>
-      <c r="E109" t="s">
-        <v>105</v>
       </c>
       <c r="F109" t="s">
         <v>42</v>
@@ -3401,24 +3935,24 @@
         <v>13</v>
       </c>
       <c r="I109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C110" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D110" t="s">
+        <v>106</v>
+      </c>
+      <c r="E110" t="s">
         <v>107</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>108</v>
-      </c>
-      <c r="F110" t="s">
-        <v>109</v>
       </c>
       <c r="G110" t="s">
         <v>13</v>
@@ -3426,25 +3960,25 @@
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C111" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D111" t="s">
+        <v>219</v>
+      </c>
+      <c r="E111" t="s">
         <v>220</v>
       </c>
-      <c r="E111" t="s">
-        <v>221</v>
-      </c>
       <c r="F111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G111" t="s">
         <v>57</v>
       </c>
       <c r="I111" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3455,10 +3989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97107629-23FF-4FFF-81A6-C8B1543F2D0F}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57:C61"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112:XFD112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3466,101 +4000,105 @@
     <col min="1" max="1" width="6.109375" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="71.88671875" customWidth="1"/>
+    <col min="5" max="5" width="69.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
         <v>129</v>
       </c>
-      <c r="D2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
         <v>131</v>
       </c>
-      <c r="D3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
         <v>133</v>
       </c>
-      <c r="D4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>39</v>
       </c>
@@ -3568,10 +4106,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>39</v>
       </c>
@@ -3579,10 +4117,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>39</v>
       </c>
@@ -3590,10 +4128,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>39</v>
       </c>
@@ -3601,32 +4139,32 @@
         <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>50</v>
       </c>
       <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>50</v>
       </c>
       <c r="C14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>54</v>
       </c>
@@ -3634,10 +4172,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>54</v>
       </c>
@@ -3645,7 +4183,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -3656,7 +4194,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -3667,7 +4205,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -3678,7 +4216,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -3689,7 +4227,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -3700,447 +4238,1639 @@
         <v>7</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="5">
         <v>2</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="5">
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="5">
         <v>4</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C31" s="5">
         <v>2</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C32" s="5">
         <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C34" s="5">
         <v>5</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C35" s="5">
         <v>6</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C36" s="5">
         <v>7</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C37" s="5">
         <v>8</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C38" s="5">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C39" s="5">
         <v>2</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C40" s="5">
         <v>3</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C41" s="5">
         <v>4</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C44" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C46" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C48" s="5">
         <v>1</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" s="5">
         <v>2</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C50" s="5">
         <v>1</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" s="5">
         <v>2</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C52" s="5">
         <v>3</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" s="5">
         <v>4</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>218</v>
+      </c>
+      <c r="C56" t="s">
         <v>168</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
-        <v>219</v>
-      </c>
-      <c r="C55" t="s">
-        <v>139</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>219</v>
-      </c>
-      <c r="C56" t="s">
-        <v>169</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C57" s="5">
         <v>1</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C58" s="5">
         <v>2</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" s="5">
         <v>3</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C60" s="5">
         <v>4</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C61" s="5">
         <v>5</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>237</v>
+      </c>
+      <c r="C62" t="s">
+        <v>238</v>
+      </c>
+      <c r="D62" t="s">
+        <v>324</v>
+      </c>
+      <c r="E62" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" t="s">
+        <v>239</v>
+      </c>
+      <c r="D63" t="s">
+        <v>325</v>
+      </c>
+      <c r="E63" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>237</v>
+      </c>
+      <c r="C64" t="s">
+        <v>240</v>
+      </c>
+      <c r="D64" t="s">
+        <v>326</v>
+      </c>
+      <c r="E64" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>237</v>
+      </c>
+      <c r="C65" t="s">
+        <v>241</v>
+      </c>
+      <c r="D65" t="s">
+        <v>327</v>
+      </c>
+      <c r="E65" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>237</v>
+      </c>
+      <c r="C66" t="s">
+        <v>242</v>
+      </c>
+      <c r="D66" t="s">
+        <v>328</v>
+      </c>
+      <c r="E66" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>237</v>
+      </c>
+      <c r="C67" t="s">
+        <v>243</v>
+      </c>
+      <c r="D67" t="s">
+        <v>329</v>
+      </c>
+      <c r="E67" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>237</v>
+      </c>
+      <c r="C68" t="s">
+        <v>244</v>
+      </c>
+      <c r="D68" t="s">
+        <v>330</v>
+      </c>
+      <c r="E68" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>237</v>
+      </c>
+      <c r="C69" t="s">
+        <v>245</v>
+      </c>
+      <c r="D69" t="s">
+        <v>331</v>
+      </c>
+      <c r="E69" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>237</v>
+      </c>
+      <c r="C70" t="s">
+        <v>246</v>
+      </c>
+      <c r="D70" t="s">
+        <v>332</v>
+      </c>
+      <c r="E70" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>237</v>
+      </c>
+      <c r="C71" t="s">
+        <v>247</v>
+      </c>
+      <c r="D71" t="s">
+        <v>333</v>
+      </c>
+      <c r="E71" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>237</v>
+      </c>
+      <c r="C72" t="s">
+        <v>248</v>
+      </c>
+      <c r="D72" t="s">
+        <v>334</v>
+      </c>
+      <c r="E72" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>237</v>
+      </c>
+      <c r="C73" t="s">
+        <v>249</v>
+      </c>
+      <c r="D73" t="s">
+        <v>335</v>
+      </c>
+      <c r="E73" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>237</v>
+      </c>
+      <c r="C74" t="s">
+        <v>250</v>
+      </c>
+      <c r="D74" t="s">
+        <v>336</v>
+      </c>
+      <c r="E74" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>237</v>
+      </c>
+      <c r="C75" t="s">
+        <v>251</v>
+      </c>
+      <c r="D75" t="s">
+        <v>337</v>
+      </c>
+      <c r="E75" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>237</v>
+      </c>
+      <c r="C76" t="s">
+        <v>252</v>
+      </c>
+      <c r="D76" t="s">
+        <v>338</v>
+      </c>
+      <c r="E76" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>237</v>
+      </c>
+      <c r="C77" t="s">
+        <v>253</v>
+      </c>
+      <c r="D77" t="s">
+        <v>330</v>
+      </c>
+      <c r="E77" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>237</v>
+      </c>
+      <c r="C78" t="s">
+        <v>254</v>
+      </c>
+      <c r="D78" t="s">
+        <v>339</v>
+      </c>
+      <c r="E78" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>237</v>
+      </c>
+      <c r="C79" t="s">
+        <v>255</v>
+      </c>
+      <c r="D79" t="s">
+        <v>340</v>
+      </c>
+      <c r="E79" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>237</v>
+      </c>
+      <c r="C80" t="s">
+        <v>256</v>
+      </c>
+      <c r="D80" t="s">
+        <v>341</v>
+      </c>
+      <c r="E80" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>237</v>
+      </c>
+      <c r="C81" t="s">
+        <v>257</v>
+      </c>
+      <c r="D81" t="s">
+        <v>342</v>
+      </c>
+      <c r="E81" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>237</v>
+      </c>
+      <c r="C82" t="s">
+        <v>258</v>
+      </c>
+      <c r="D82" t="s">
+        <v>343</v>
+      </c>
+      <c r="E82" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>237</v>
+      </c>
+      <c r="C83" t="s">
+        <v>259</v>
+      </c>
+      <c r="D83" t="s">
+        <v>344</v>
+      </c>
+      <c r="E83" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>237</v>
+      </c>
+      <c r="C84" t="s">
+        <v>260</v>
+      </c>
+      <c r="D84" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>237</v>
+      </c>
+      <c r="C85" t="s">
+        <v>261</v>
+      </c>
+      <c r="D85" t="s">
+        <v>346</v>
+      </c>
+      <c r="E85" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>237</v>
+      </c>
+      <c r="C86" t="s">
+        <v>262</v>
+      </c>
+      <c r="D86" t="s">
+        <v>347</v>
+      </c>
+      <c r="E86" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>237</v>
+      </c>
+      <c r="C87" t="s">
+        <v>263</v>
+      </c>
+      <c r="D87" t="s">
+        <v>348</v>
+      </c>
+      <c r="E87" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>237</v>
+      </c>
+      <c r="C88" t="s">
+        <v>264</v>
+      </c>
+      <c r="D88" t="s">
+        <v>349</v>
+      </c>
+      <c r="E88" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>237</v>
+      </c>
+      <c r="C89" t="s">
+        <v>265</v>
+      </c>
+      <c r="D89" t="s">
+        <v>350</v>
+      </c>
+      <c r="E89" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>237</v>
+      </c>
+      <c r="C90" t="s">
+        <v>266</v>
+      </c>
+      <c r="D90" t="s">
+        <v>351</v>
+      </c>
+      <c r="E90" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>237</v>
+      </c>
+      <c r="C91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D91" t="s">
+        <v>352</v>
+      </c>
+      <c r="E91" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>237</v>
+      </c>
+      <c r="C92" t="s">
+        <v>268</v>
+      </c>
+      <c r="D92" t="s">
+        <v>353</v>
+      </c>
+      <c r="E92" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>237</v>
+      </c>
+      <c r="C93" t="s">
+        <v>269</v>
+      </c>
+      <c r="D93" t="s">
+        <v>354</v>
+      </c>
+      <c r="E93" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>237</v>
+      </c>
+      <c r="C94" t="s">
+        <v>270</v>
+      </c>
+      <c r="D94" t="s">
+        <v>355</v>
+      </c>
+      <c r="E94" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>237</v>
+      </c>
+      <c r="C95" t="s">
+        <v>271</v>
+      </c>
+      <c r="D95" t="s">
+        <v>356</v>
+      </c>
+      <c r="E95" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>237</v>
+      </c>
+      <c r="C96" t="s">
+        <v>272</v>
+      </c>
+      <c r="D96" t="s">
+        <v>357</v>
+      </c>
+      <c r="E96" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>237</v>
+      </c>
+      <c r="C97" t="s">
+        <v>273</v>
+      </c>
+      <c r="D97" t="s">
+        <v>358</v>
+      </c>
+      <c r="E97" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>237</v>
+      </c>
+      <c r="C98" t="s">
+        <v>274</v>
+      </c>
+      <c r="D98" t="s">
+        <v>359</v>
+      </c>
+      <c r="E98" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>237</v>
+      </c>
+      <c r="C99" t="s">
+        <v>275</v>
+      </c>
+      <c r="D99" t="s">
+        <v>360</v>
+      </c>
+      <c r="E99" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>237</v>
+      </c>
+      <c r="C100" t="s">
+        <v>276</v>
+      </c>
+      <c r="D100" t="s">
+        <v>361</v>
+      </c>
+      <c r="E100" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>237</v>
+      </c>
+      <c r="C101" t="s">
+        <v>277</v>
+      </c>
+      <c r="D101" t="s">
+        <v>362</v>
+      </c>
+      <c r="E101" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>237</v>
+      </c>
+      <c r="C102" t="s">
+        <v>278</v>
+      </c>
+      <c r="D102" t="s">
+        <v>363</v>
+      </c>
+      <c r="E102" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>237</v>
+      </c>
+      <c r="C103" t="s">
+        <v>279</v>
+      </c>
+      <c r="D103" t="s">
+        <v>364</v>
+      </c>
+      <c r="E103" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>237</v>
+      </c>
+      <c r="C104" t="s">
+        <v>280</v>
+      </c>
+      <c r="D104" t="s">
+        <v>405</v>
+      </c>
+      <c r="E104" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>237</v>
+      </c>
+      <c r="C105" t="s">
+        <v>281</v>
+      </c>
+      <c r="D105" t="s">
+        <v>365</v>
+      </c>
+      <c r="E105" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>237</v>
+      </c>
+      <c r="C106" t="s">
+        <v>282</v>
+      </c>
+      <c r="D106" t="s">
+        <v>366</v>
+      </c>
+      <c r="E106" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>237</v>
+      </c>
+      <c r="C107" t="s">
+        <v>283</v>
+      </c>
+      <c r="D107" t="s">
+        <v>367</v>
+      </c>
+      <c r="E107" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>237</v>
+      </c>
+      <c r="C108" t="s">
+        <v>284</v>
+      </c>
+      <c r="D108" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>237</v>
+      </c>
+      <c r="C109" t="s">
+        <v>285</v>
+      </c>
+      <c r="D109" t="s">
+        <v>325</v>
+      </c>
+      <c r="E109" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>237</v>
+      </c>
+      <c r="C110" t="s">
+        <v>286</v>
+      </c>
+      <c r="D110" t="s">
+        <v>369</v>
+      </c>
+      <c r="E110" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>237</v>
+      </c>
+      <c r="C111" t="s">
+        <v>287</v>
+      </c>
+      <c r="D111" t="s">
+        <v>370</v>
+      </c>
+      <c r="E111" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>237</v>
+      </c>
+      <c r="C112" t="s">
+        <v>288</v>
+      </c>
+      <c r="D112" t="s">
+        <v>371</v>
+      </c>
+      <c r="E112" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>237</v>
+      </c>
+      <c r="C113" t="s">
+        <v>289</v>
+      </c>
+      <c r="D113" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>237</v>
+      </c>
+      <c r="C114" t="s">
+        <v>290</v>
+      </c>
+      <c r="D114" t="s">
+        <v>373</v>
+      </c>
+      <c r="E114" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>237</v>
+      </c>
+      <c r="C115" t="s">
+        <v>291</v>
+      </c>
+      <c r="D115" t="s">
+        <v>350</v>
+      </c>
+      <c r="E115" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>237</v>
+      </c>
+      <c r="C116" t="s">
+        <v>292</v>
+      </c>
+      <c r="D116" t="s">
+        <v>374</v>
+      </c>
+      <c r="E116" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>237</v>
+      </c>
+      <c r="C117" t="s">
+        <v>293</v>
+      </c>
+      <c r="D117" t="s">
+        <v>375</v>
+      </c>
+      <c r="E117" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>237</v>
+      </c>
+      <c r="C118" t="s">
+        <v>294</v>
+      </c>
+      <c r="D118" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>237</v>
+      </c>
+      <c r="C119" t="s">
+        <v>295</v>
+      </c>
+      <c r="D119" t="s">
+        <v>377</v>
+      </c>
+      <c r="E119" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>237</v>
+      </c>
+      <c r="C120" t="s">
+        <v>296</v>
+      </c>
+      <c r="D120" t="s">
+        <v>378</v>
+      </c>
+      <c r="E120" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>237</v>
+      </c>
+      <c r="C121" t="s">
+        <v>297</v>
+      </c>
+      <c r="D121" t="s">
+        <v>379</v>
+      </c>
+      <c r="E121" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>237</v>
+      </c>
+      <c r="C122" t="s">
+        <v>298</v>
+      </c>
+      <c r="D122" t="s">
+        <v>380</v>
+      </c>
+      <c r="E122" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>237</v>
+      </c>
+      <c r="C123" t="s">
+        <v>299</v>
+      </c>
+      <c r="D123" t="s">
+        <v>381</v>
+      </c>
+      <c r="E123" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>237</v>
+      </c>
+      <c r="C124" t="s">
+        <v>300</v>
+      </c>
+      <c r="D124" t="s">
+        <v>382</v>
+      </c>
+      <c r="E124" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>237</v>
+      </c>
+      <c r="C125" t="s">
+        <v>301</v>
+      </c>
+      <c r="D125" t="s">
+        <v>383</v>
+      </c>
+      <c r="E125" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>237</v>
+      </c>
+      <c r="C126" t="s">
+        <v>302</v>
+      </c>
+      <c r="D126" t="s">
+        <v>384</v>
+      </c>
+      <c r="E126" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>237</v>
+      </c>
+      <c r="C127" t="s">
+        <v>303</v>
+      </c>
+      <c r="D127" t="s">
+        <v>385</v>
+      </c>
+      <c r="E127" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>237</v>
+      </c>
+      <c r="C128" t="s">
+        <v>304</v>
+      </c>
+      <c r="D128" t="s">
+        <v>386</v>
+      </c>
+      <c r="E128" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>237</v>
+      </c>
+      <c r="C129" t="s">
+        <v>305</v>
+      </c>
+      <c r="D129" t="s">
+        <v>387</v>
+      </c>
+      <c r="E129" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>237</v>
+      </c>
+      <c r="C130" t="s">
+        <v>306</v>
+      </c>
+      <c r="D130" t="s">
+        <v>388</v>
+      </c>
+      <c r="E130" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>237</v>
+      </c>
+      <c r="C131" t="s">
+        <v>307</v>
+      </c>
+      <c r="D131" t="s">
+        <v>389</v>
+      </c>
+      <c r="E131" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>237</v>
+      </c>
+      <c r="C132" t="s">
+        <v>308</v>
+      </c>
+      <c r="D132" t="s">
+        <v>390</v>
+      </c>
+      <c r="E132" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>237</v>
+      </c>
+      <c r="C133" t="s">
+        <v>309</v>
+      </c>
+      <c r="D133" t="s">
+        <v>391</v>
+      </c>
+      <c r="E133" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>237</v>
+      </c>
+      <c r="C134" t="s">
+        <v>310</v>
+      </c>
+      <c r="D134" t="s">
+        <v>392</v>
+      </c>
+      <c r="E134" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>237</v>
+      </c>
+      <c r="C135" t="s">
+        <v>311</v>
+      </c>
+      <c r="D135" t="s">
+        <v>393</v>
+      </c>
+      <c r="E135" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>237</v>
+      </c>
+      <c r="C136" t="s">
+        <v>312</v>
+      </c>
+      <c r="D136" t="s">
+        <v>394</v>
+      </c>
+      <c r="E136" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>237</v>
+      </c>
+      <c r="C137" t="s">
+        <v>313</v>
+      </c>
+      <c r="D137" t="s">
+        <v>395</v>
+      </c>
+      <c r="E137" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>237</v>
+      </c>
+      <c r="C138" t="s">
+        <v>314</v>
+      </c>
+      <c r="D138" t="s">
+        <v>406</v>
+      </c>
+      <c r="E138" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>237</v>
+      </c>
+      <c r="C139" t="s">
+        <v>315</v>
+      </c>
+      <c r="D139" t="s">
+        <v>396</v>
+      </c>
+      <c r="E139" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>237</v>
+      </c>
+      <c r="C140" t="s">
+        <v>316</v>
+      </c>
+      <c r="D140" t="s">
+        <v>397</v>
+      </c>
+      <c r="E140" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>237</v>
+      </c>
+      <c r="C141" t="s">
+        <v>317</v>
+      </c>
+      <c r="D141" t="s">
+        <v>398</v>
+      </c>
+      <c r="E141" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>237</v>
+      </c>
+      <c r="C142" t="s">
+        <v>318</v>
+      </c>
+      <c r="D142" t="s">
+        <v>399</v>
+      </c>
+      <c r="E142" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>237</v>
+      </c>
+      <c r="C143" t="s">
+        <v>319</v>
+      </c>
+      <c r="D143" t="s">
+        <v>400</v>
+      </c>
+      <c r="E143" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>237</v>
+      </c>
+      <c r="C144" t="s">
+        <v>320</v>
+      </c>
+      <c r="D144" t="s">
+        <v>401</v>
+      </c>
+      <c r="E144" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>237</v>
+      </c>
+      <c r="C145" t="s">
+        <v>321</v>
+      </c>
+      <c r="D145" t="s">
+        <v>402</v>
+      </c>
+      <c r="E145" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>237</v>
+      </c>
+      <c r="C146" t="s">
+        <v>322</v>
+      </c>
+      <c r="D146" t="s">
+        <v>403</v>
+      </c>
+      <c r="E146" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>237</v>
+      </c>
+      <c r="C147" t="s">
+        <v>323</v>
+      </c>
+      <c r="D147" t="s">
+        <v>404</v>
+      </c>
+      <c r="E147" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dedup of ARV_REGIMEN codes. Bump Data Dictionary with fixes up to draft v1.5
</commit_message>
<xml_diff>
--- a/files_and_resources/Data Dictionary.xlsx
+++ b/files_and_resources/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubarak Abdu-Aguye\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB224EB2-96D5-48C2-A2BF-BEE64F6AEF67}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49DEF55-4895-4323-B660-F1872FA6E461}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="380">
   <si>
     <t>ID</t>
   </si>
@@ -745,9 +745,6 @@
     <t>The name of the PCR lab sending/returning the results</t>
   </si>
   <si>
-    <t>ARV_REGIMEN</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
@@ -793,9 +790,6 @@
     <t>1s</t>
   </si>
   <si>
-    <t>1t</t>
-  </si>
-  <si>
     <t>1u</t>
   </si>
   <si>
@@ -889,54 +883,6 @@
     <t>2g</t>
   </si>
   <si>
-    <t>4b</t>
-  </si>
-  <si>
-    <t>4c</t>
-  </si>
-  <si>
-    <t>4d</t>
-  </si>
-  <si>
-    <t>4f</t>
-  </si>
-  <si>
-    <t>4g</t>
-  </si>
-  <si>
-    <t>5a</t>
-  </si>
-  <si>
-    <t>5b</t>
-  </si>
-  <si>
-    <t>5c</t>
-  </si>
-  <si>
-    <t>5d</t>
-  </si>
-  <si>
-    <t>5f</t>
-  </si>
-  <si>
-    <t>6a</t>
-  </si>
-  <si>
-    <t>6b</t>
-  </si>
-  <si>
-    <t>6c</t>
-  </si>
-  <si>
-    <t>6d</t>
-  </si>
-  <si>
-    <t>6e</t>
-  </si>
-  <si>
-    <t>6f</t>
-  </si>
-  <si>
     <t>3a</t>
   </si>
   <si>
@@ -1027,9 +973,6 @@
     <t>ABC-3TC-AZT</t>
   </si>
   <si>
-    <t>TDF-3TC-AZT</t>
-  </si>
-  <si>
     <t>TDF-3TC-DTG</t>
   </si>
   <si>
@@ -1141,48 +1084,6 @@
     <t>Adult Second Line Others</t>
   </si>
   <si>
-    <t>ABC-3TC-EFV</t>
-  </si>
-  <si>
-    <t>ABC-3TC-NVP</t>
-  </si>
-  <si>
-    <t>d4T-3TC-NVP</t>
-  </si>
-  <si>
-    <t>Child First Line Others</t>
-  </si>
-  <si>
-    <t>ABC-3TC-LPV/r</t>
-  </si>
-  <si>
-    <t>d4T-3TC-LPV/r</t>
-  </si>
-  <si>
-    <t>ddi-3TC-NVP</t>
-  </si>
-  <si>
-    <t>Child Second Line Others</t>
-  </si>
-  <si>
-    <t>DRV/r + 2 NRTIs + 2 NNRTI</t>
-  </si>
-  <si>
-    <t>DRV/r +2NRTIs</t>
-  </si>
-  <si>
-    <t>DRV/r-DTG + 1-2 NRTIs</t>
-  </si>
-  <si>
-    <t>DRV/r+RAL + 1-2NRTIs</t>
-  </si>
-  <si>
-    <t>DTG+2 NRTIs</t>
-  </si>
-  <si>
-    <t>RAL(or DTG) + 2 NRTIs</t>
-  </si>
-  <si>
     <t>AZT-TDF-3TC-LPV/r</t>
   </si>
   <si>
@@ -1264,19 +1165,13 @@
     <t>Adult 2nd line ARV regimen</t>
   </si>
   <si>
-    <t xml:space="preserve"> Adult 1st line ARV regimen/ Child 1st line ARV regimen</t>
-  </si>
-  <si>
-    <t>Child 1st line ARV regimen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Child 2nd line ARV regimen</t>
-  </si>
-  <si>
-    <t>Child 3rd Line ARV Regimens</t>
-  </si>
-  <si>
     <t>Adult 3rd Line ARV Regimens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDF-3TC-AZT </t>
+  </si>
+  <si>
+    <t>ARV_REGIMEN_ADULT</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1386,6 +1281,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1702,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7068A318-C14F-4D04-B583-D7B1DF373F65}">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1715,7 +1611,7 @@
     <col min="5" max="5" width="33.109375" customWidth="1"/>
     <col min="6" max="6" width="11.21875" customWidth="1"/>
     <col min="7" max="7" width="7.109375" customWidth="1"/>
-    <col min="8" max="8" width="67.21875" customWidth="1"/>
+    <col min="8" max="8" width="57.88671875" customWidth="1"/>
     <col min="9" max="9" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2129,7 +2025,7 @@
         <v>57</v>
       </c>
       <c r="I19" t="s">
-        <v>237</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
@@ -3989,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97107629-23FF-4FFF-81A6-C8B1543F2D0F}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:XFD112"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62:B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4018,7 +3914,7 @@
         <v>127</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>407</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4683,1197 +4579,966 @@
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
+        <v>379</v>
+      </c>
+      <c r="C62" t="s">
         <v>237</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
+        <v>306</v>
+      </c>
+      <c r="E62" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C63" t="s">
         <v>238</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
+        <v>307</v>
+      </c>
+      <c r="E63" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C64" t="s">
+        <v>239</v>
+      </c>
+      <c r="D64" t="s">
+        <v>308</v>
+      </c>
+      <c r="E64" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C65" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" t="s">
+        <v>309</v>
+      </c>
+      <c r="E65" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C66" t="s">
+        <v>241</v>
+      </c>
+      <c r="D66" t="s">
+        <v>310</v>
+      </c>
+      <c r="E66" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C67" t="s">
+        <v>242</v>
+      </c>
+      <c r="D67" t="s">
+        <v>311</v>
+      </c>
+      <c r="E67" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C68" t="s">
+        <v>243</v>
+      </c>
+      <c r="D68" t="s">
+        <v>312</v>
+      </c>
+      <c r="E68" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B69" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C69" t="s">
+        <v>244</v>
+      </c>
+      <c r="D69" t="s">
+        <v>378</v>
+      </c>
+      <c r="E69" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C70" t="s">
+        <v>245</v>
+      </c>
+      <c r="D70" t="s">
+        <v>313</v>
+      </c>
+      <c r="E70" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C71" t="s">
+        <v>246</v>
+      </c>
+      <c r="D71" t="s">
+        <v>314</v>
+      </c>
+      <c r="E71" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C72" t="s">
+        <v>247</v>
+      </c>
+      <c r="D72" t="s">
+        <v>315</v>
+      </c>
+      <c r="E72" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C73" t="s">
+        <v>248</v>
+      </c>
+      <c r="D73" t="s">
+        <v>316</v>
+      </c>
+      <c r="E73" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C74" t="s">
+        <v>249</v>
+      </c>
+      <c r="D74" t="s">
+        <v>317</v>
+      </c>
+      <c r="E74" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C75" t="s">
+        <v>250</v>
+      </c>
+      <c r="D75" t="s">
+        <v>318</v>
+      </c>
+      <c r="E75" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B76" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C76" t="s">
+        <v>251</v>
+      </c>
+      <c r="D76" t="s">
+        <v>319</v>
+      </c>
+      <c r="E76" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B77" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C77" t="s">
+        <v>252</v>
+      </c>
+      <c r="D77" t="s">
+        <v>320</v>
+      </c>
+      <c r="E77" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B78" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C78" t="s">
+        <v>253</v>
+      </c>
+      <c r="D78" t="s">
+        <v>321</v>
+      </c>
+      <c r="E78" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C79" t="s">
+        <v>254</v>
+      </c>
+      <c r="D79" t="s">
+        <v>322</v>
+      </c>
+      <c r="E79" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B80" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C80" t="s">
+        <v>255</v>
+      </c>
+      <c r="D80" t="s">
+        <v>323</v>
+      </c>
+      <c r="E80" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B81" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C81" t="s">
+        <v>256</v>
+      </c>
+      <c r="D81" t="s">
         <v>324</v>
       </c>
-      <c r="E62" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
-        <v>237</v>
-      </c>
-      <c r="C63" t="s">
-        <v>239</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E81" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B82" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C82" t="s">
+        <v>257</v>
+      </c>
+      <c r="D82" t="s">
         <v>325</v>
       </c>
-      <c r="E63" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
-        <v>237</v>
-      </c>
-      <c r="C64" t="s">
-        <v>240</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E82" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B83" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C83" t="s">
+        <v>258</v>
+      </c>
+      <c r="D83" t="s">
         <v>326</v>
       </c>
-      <c r="E64" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
-        <v>237</v>
-      </c>
-      <c r="C65" t="s">
-        <v>241</v>
-      </c>
-      <c r="D65" t="s">
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B84" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C84" t="s">
+        <v>259</v>
+      </c>
+      <c r="D84" t="s">
         <v>327</v>
       </c>
-      <c r="E65" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
-        <v>237</v>
-      </c>
-      <c r="C66" t="s">
-        <v>242</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="E84" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B85" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C85" t="s">
+        <v>260</v>
+      </c>
+      <c r="D85" t="s">
         <v>328</v>
       </c>
-      <c r="E66" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
-        <v>237</v>
-      </c>
-      <c r="C67" t="s">
-        <v>243</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E85" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B86" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C86" t="s">
+        <v>261</v>
+      </c>
+      <c r="D86" t="s">
         <v>329</v>
       </c>
-      <c r="E67" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
-        <v>237</v>
-      </c>
-      <c r="C68" t="s">
-        <v>244</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E86" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C87" t="s">
+        <v>262</v>
+      </c>
+      <c r="D87" t="s">
         <v>330</v>
       </c>
-      <c r="E68" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
-        <v>237</v>
-      </c>
-      <c r="C69" t="s">
-        <v>245</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E87" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C88" t="s">
+        <v>263</v>
+      </c>
+      <c r="D88" t="s">
         <v>331</v>
       </c>
-      <c r="E69" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
-        <v>237</v>
-      </c>
-      <c r="C70" t="s">
-        <v>246</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="E88" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B89" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C89" t="s">
+        <v>264</v>
+      </c>
+      <c r="D89" t="s">
         <v>332</v>
       </c>
-      <c r="E70" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
-        <v>237</v>
-      </c>
-      <c r="C71" t="s">
-        <v>247</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E89" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B90" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C90" t="s">
+        <v>265</v>
+      </c>
+      <c r="D90" t="s">
         <v>333</v>
       </c>
-      <c r="E71" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
-        <v>237</v>
-      </c>
-      <c r="C72" t="s">
-        <v>248</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="E90" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B91" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C91" t="s">
+        <v>266</v>
+      </c>
+      <c r="D91" t="s">
         <v>334</v>
       </c>
-      <c r="E72" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
-        <v>237</v>
-      </c>
-      <c r="C73" t="s">
-        <v>249</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="E91" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C92" t="s">
+        <v>267</v>
+      </c>
+      <c r="D92" t="s">
         <v>335</v>
       </c>
-      <c r="E73" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
-        <v>237</v>
-      </c>
-      <c r="C74" t="s">
-        <v>250</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="E92" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C93" t="s">
+        <v>268</v>
+      </c>
+      <c r="D93" t="s">
         <v>336</v>
       </c>
-      <c r="E74" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>237</v>
-      </c>
-      <c r="C75" t="s">
-        <v>251</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="E93" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C94" t="s">
+        <v>269</v>
+      </c>
+      <c r="D94" t="s">
         <v>337</v>
       </c>
-      <c r="E75" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
-        <v>237</v>
-      </c>
-      <c r="C76" t="s">
-        <v>252</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E94" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B95" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C95" t="s">
+        <v>270</v>
+      </c>
+      <c r="D95" t="s">
         <v>338</v>
       </c>
-      <c r="E76" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>237</v>
-      </c>
-      <c r="C77" t="s">
-        <v>253</v>
-      </c>
-      <c r="D77" t="s">
-        <v>330</v>
-      </c>
-      <c r="E77" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
-        <v>237</v>
-      </c>
-      <c r="C78" t="s">
-        <v>254</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="E95" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B96" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C96" t="s">
+        <v>271</v>
+      </c>
+      <c r="D96" t="s">
         <v>339</v>
       </c>
-      <c r="E78" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>237</v>
-      </c>
-      <c r="C79" t="s">
-        <v>255</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="E96" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B97" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C97" t="s">
+        <v>272</v>
+      </c>
+      <c r="D97" t="s">
         <v>340</v>
       </c>
-      <c r="E79" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>237</v>
-      </c>
-      <c r="C80" t="s">
-        <v>256</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="E97" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B98" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C98" t="s">
+        <v>273</v>
+      </c>
+      <c r="D98" t="s">
         <v>341</v>
       </c>
-      <c r="E80" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
-        <v>237</v>
-      </c>
-      <c r="C81" t="s">
-        <v>257</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E98" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B99" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C99" t="s">
+        <v>274</v>
+      </c>
+      <c r="D99" t="s">
         <v>342</v>
       </c>
-      <c r="E81" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
-        <v>237</v>
-      </c>
-      <c r="C82" t="s">
-        <v>258</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E99" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B100" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C100" t="s">
+        <v>275</v>
+      </c>
+      <c r="D100" t="s">
         <v>343</v>
       </c>
-      <c r="E82" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>237</v>
-      </c>
-      <c r="C83" t="s">
-        <v>259</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E100" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B101" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C101" t="s">
+        <v>276</v>
+      </c>
+      <c r="D101" t="s">
         <v>344</v>
       </c>
-      <c r="E83" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
-        <v>237</v>
-      </c>
-      <c r="C84" t="s">
-        <v>260</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E101" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B102" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C102" t="s">
+        <v>277</v>
+      </c>
+      <c r="D102" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B85" t="s">
-        <v>237</v>
-      </c>
-      <c r="C85" t="s">
-        <v>261</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E102" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B103" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C103" t="s">
+        <v>278</v>
+      </c>
+      <c r="D103" t="s">
+        <v>372</v>
+      </c>
+      <c r="E103" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B104" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C104" t="s">
+        <v>279</v>
+      </c>
+      <c r="D104" t="s">
         <v>346</v>
       </c>
-      <c r="E85" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>237</v>
-      </c>
-      <c r="C86" t="s">
-        <v>262</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E104" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B105" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C105" t="s">
+        <v>280</v>
+      </c>
+      <c r="D105" t="s">
         <v>347</v>
       </c>
-      <c r="E86" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B87" t="s">
-        <v>237</v>
-      </c>
-      <c r="C87" t="s">
-        <v>263</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E105" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B106" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C106" t="s">
+        <v>281</v>
+      </c>
+      <c r="D106" t="s">
         <v>348</v>
       </c>
-      <c r="E87" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
-        <v>237</v>
-      </c>
-      <c r="C88" t="s">
-        <v>264</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E106" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B107" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C107" t="s">
+        <v>282</v>
+      </c>
+      <c r="D107" t="s">
         <v>349</v>
       </c>
-      <c r="E88" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
-        <v>237</v>
-      </c>
-      <c r="C89" t="s">
-        <v>265</v>
-      </c>
-      <c r="D89" t="s">
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B108" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C108" t="s">
+        <v>283</v>
+      </c>
+      <c r="D108" t="s">
         <v>350</v>
       </c>
-      <c r="E89" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
-        <v>237</v>
-      </c>
-      <c r="C90" t="s">
-        <v>266</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E108" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B109" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C109" t="s">
+        <v>284</v>
+      </c>
+      <c r="D109" t="s">
         <v>351</v>
       </c>
-      <c r="E90" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
-        <v>237</v>
-      </c>
-      <c r="C91" t="s">
-        <v>267</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E109" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B110" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C110" t="s">
+        <v>285</v>
+      </c>
+      <c r="D110" t="s">
         <v>352</v>
       </c>
-      <c r="E91" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B92" t="s">
-        <v>237</v>
-      </c>
-      <c r="C92" t="s">
-        <v>268</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E110" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B111" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C111" t="s">
+        <v>286</v>
+      </c>
+      <c r="D111" t="s">
         <v>353</v>
       </c>
-      <c r="E92" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B93" t="s">
-        <v>237</v>
-      </c>
-      <c r="C93" t="s">
-        <v>269</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E111" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B112" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C112" t="s">
+        <v>287</v>
+      </c>
+      <c r="D112" t="s">
         <v>354</v>
       </c>
-      <c r="E93" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
-        <v>237</v>
-      </c>
-      <c r="C94" t="s">
-        <v>270</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E112" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B113" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C113" t="s">
+        <v>288</v>
+      </c>
+      <c r="D113" t="s">
         <v>355</v>
       </c>
-      <c r="E94" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B95" t="s">
-        <v>237</v>
-      </c>
-      <c r="C95" t="s">
-        <v>271</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E113" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B114" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C114" t="s">
+        <v>289</v>
+      </c>
+      <c r="D114" t="s">
         <v>356</v>
       </c>
-      <c r="E95" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B96" t="s">
-        <v>237</v>
-      </c>
-      <c r="C96" t="s">
-        <v>272</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="E114" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B115" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C115" t="s">
+        <v>290</v>
+      </c>
+      <c r="D115" t="s">
         <v>357</v>
       </c>
-      <c r="E96" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
-        <v>237</v>
-      </c>
-      <c r="C97" t="s">
-        <v>273</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="E115" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B116" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C116" t="s">
+        <v>291</v>
+      </c>
+      <c r="D116" t="s">
         <v>358</v>
       </c>
-      <c r="E97" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B98" t="s">
-        <v>237</v>
-      </c>
-      <c r="C98" t="s">
-        <v>274</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E116" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B117" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C117" t="s">
+        <v>292</v>
+      </c>
+      <c r="D117" t="s">
         <v>359</v>
       </c>
-      <c r="E98" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
-        <v>237</v>
-      </c>
-      <c r="C99" t="s">
-        <v>275</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E117" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B118" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C118" t="s">
+        <v>293</v>
+      </c>
+      <c r="D118" t="s">
         <v>360</v>
       </c>
-      <c r="E99" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B100" t="s">
-        <v>237</v>
-      </c>
-      <c r="C100" t="s">
-        <v>276</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="E118" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B119" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C119" t="s">
+        <v>294</v>
+      </c>
+      <c r="D119" t="s">
         <v>361</v>
       </c>
-      <c r="E100" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B101" t="s">
-        <v>237</v>
-      </c>
-      <c r="C101" t="s">
-        <v>277</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="E119" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B120" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C120" t="s">
+        <v>295</v>
+      </c>
+      <c r="D120" t="s">
         <v>362</v>
       </c>
-      <c r="E101" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B102" t="s">
-        <v>237</v>
-      </c>
-      <c r="C102" t="s">
-        <v>278</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="E120" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B121" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C121" t="s">
+        <v>296</v>
+      </c>
+      <c r="D121" t="s">
+        <v>373</v>
+      </c>
+      <c r="E121" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B122" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C122" t="s">
+        <v>297</v>
+      </c>
+      <c r="D122" t="s">
         <v>363</v>
       </c>
-      <c r="E102" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B103" t="s">
-        <v>237</v>
-      </c>
-      <c r="C103" t="s">
-        <v>279</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="E122" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B123" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C123" t="s">
+        <v>298</v>
+      </c>
+      <c r="D123" t="s">
         <v>364</v>
       </c>
-      <c r="E103" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
-        <v>237</v>
-      </c>
-      <c r="C104" t="s">
-        <v>280</v>
-      </c>
-      <c r="D104" t="s">
-        <v>405</v>
-      </c>
-      <c r="E104" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B105" t="s">
-        <v>237</v>
-      </c>
-      <c r="C105" t="s">
-        <v>281</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="E123" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B124" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C124" t="s">
+        <v>299</v>
+      </c>
+      <c r="D124" t="s">
         <v>365</v>
       </c>
-      <c r="E105" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B106" t="s">
-        <v>237</v>
-      </c>
-      <c r="C106" t="s">
-        <v>282</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="E124" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B125" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C125" t="s">
+        <v>300</v>
+      </c>
+      <c r="D125" t="s">
         <v>366</v>
       </c>
-      <c r="E106" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B107" t="s">
-        <v>237</v>
-      </c>
-      <c r="C107" t="s">
-        <v>283</v>
-      </c>
-      <c r="D107" t="s">
+      <c r="E125" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B126" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C126" t="s">
+        <v>301</v>
+      </c>
+      <c r="D126" t="s">
         <v>367</v>
       </c>
-      <c r="E107" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B108" t="s">
-        <v>237</v>
-      </c>
-      <c r="C108" t="s">
-        <v>284</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="E126" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B127" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C127" t="s">
+        <v>302</v>
+      </c>
+      <c r="D127" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B109" t="s">
-        <v>237</v>
-      </c>
-      <c r="C109" t="s">
-        <v>285</v>
-      </c>
-      <c r="D109" t="s">
-        <v>325</v>
-      </c>
-      <c r="E109" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B110" t="s">
-        <v>237</v>
-      </c>
-      <c r="C110" t="s">
-        <v>286</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="E127" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B128" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C128" t="s">
+        <v>303</v>
+      </c>
+      <c r="D128" t="s">
         <v>369</v>
       </c>
-      <c r="E110" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B111" t="s">
-        <v>237</v>
-      </c>
-      <c r="C111" t="s">
-        <v>287</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="E128" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B129" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C129" t="s">
+        <v>304</v>
+      </c>
+      <c r="D129" t="s">
         <v>370</v>
       </c>
-      <c r="E111" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B112" t="s">
-        <v>237</v>
-      </c>
-      <c r="C112" t="s">
-        <v>288</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="E129" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B130" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C130" t="s">
+        <v>305</v>
+      </c>
+      <c r="D130" t="s">
         <v>371</v>
       </c>
-      <c r="E112" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B113" t="s">
-        <v>237</v>
-      </c>
-      <c r="C113" t="s">
-        <v>289</v>
-      </c>
-      <c r="D113" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B114" t="s">
-        <v>237</v>
-      </c>
-      <c r="C114" t="s">
-        <v>290</v>
-      </c>
-      <c r="D114" t="s">
-        <v>373</v>
-      </c>
-      <c r="E114" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B115" t="s">
-        <v>237</v>
-      </c>
-      <c r="C115" t="s">
-        <v>291</v>
-      </c>
-      <c r="D115" t="s">
-        <v>350</v>
-      </c>
-      <c r="E115" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B116" t="s">
-        <v>237</v>
-      </c>
-      <c r="C116" t="s">
-        <v>292</v>
-      </c>
-      <c r="D116" t="s">
-        <v>374</v>
-      </c>
-      <c r="E116" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B117" t="s">
-        <v>237</v>
-      </c>
-      <c r="C117" t="s">
-        <v>293</v>
-      </c>
-      <c r="D117" t="s">
-        <v>375</v>
-      </c>
-      <c r="E117" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B118" t="s">
-        <v>237</v>
-      </c>
-      <c r="C118" t="s">
-        <v>294</v>
-      </c>
-      <c r="D118" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B119" t="s">
-        <v>237</v>
-      </c>
-      <c r="C119" t="s">
-        <v>295</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="E130" t="s">
         <v>377</v>
-      </c>
-      <c r="E119" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
-        <v>237</v>
-      </c>
-      <c r="C120" t="s">
-        <v>296</v>
-      </c>
-      <c r="D120" t="s">
-        <v>378</v>
-      </c>
-      <c r="E120" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B121" t="s">
-        <v>237</v>
-      </c>
-      <c r="C121" t="s">
-        <v>297</v>
-      </c>
-      <c r="D121" t="s">
-        <v>379</v>
-      </c>
-      <c r="E121" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B122" t="s">
-        <v>237</v>
-      </c>
-      <c r="C122" t="s">
-        <v>298</v>
-      </c>
-      <c r="D122" t="s">
-        <v>380</v>
-      </c>
-      <c r="E122" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B123" t="s">
-        <v>237</v>
-      </c>
-      <c r="C123" t="s">
-        <v>299</v>
-      </c>
-      <c r="D123" t="s">
-        <v>381</v>
-      </c>
-      <c r="E123" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
-        <v>237</v>
-      </c>
-      <c r="C124" t="s">
-        <v>300</v>
-      </c>
-      <c r="D124" t="s">
-        <v>382</v>
-      </c>
-      <c r="E124" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B125" t="s">
-        <v>237</v>
-      </c>
-      <c r="C125" t="s">
-        <v>301</v>
-      </c>
-      <c r="D125" t="s">
-        <v>383</v>
-      </c>
-      <c r="E125" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B126" t="s">
-        <v>237</v>
-      </c>
-      <c r="C126" t="s">
-        <v>302</v>
-      </c>
-      <c r="D126" t="s">
-        <v>384</v>
-      </c>
-      <c r="E126" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
-        <v>237</v>
-      </c>
-      <c r="C127" t="s">
-        <v>303</v>
-      </c>
-      <c r="D127" t="s">
-        <v>385</v>
-      </c>
-      <c r="E127" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B128" t="s">
-        <v>237</v>
-      </c>
-      <c r="C128" t="s">
-        <v>304</v>
-      </c>
-      <c r="D128" t="s">
-        <v>386</v>
-      </c>
-      <c r="E128" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B129" t="s">
-        <v>237</v>
-      </c>
-      <c r="C129" t="s">
-        <v>305</v>
-      </c>
-      <c r="D129" t="s">
-        <v>387</v>
-      </c>
-      <c r="E129" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B130" t="s">
-        <v>237</v>
-      </c>
-      <c r="C130" t="s">
-        <v>306</v>
-      </c>
-      <c r="D130" t="s">
-        <v>388</v>
-      </c>
-      <c r="E130" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B131" t="s">
-        <v>237</v>
-      </c>
-      <c r="C131" t="s">
-        <v>307</v>
-      </c>
-      <c r="D131" t="s">
-        <v>389</v>
-      </c>
-      <c r="E131" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B132" t="s">
-        <v>237</v>
-      </c>
-      <c r="C132" t="s">
-        <v>308</v>
-      </c>
-      <c r="D132" t="s">
-        <v>390</v>
-      </c>
-      <c r="E132" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B133" t="s">
-        <v>237</v>
-      </c>
-      <c r="C133" t="s">
-        <v>309</v>
-      </c>
-      <c r="D133" t="s">
-        <v>391</v>
-      </c>
-      <c r="E133" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B134" t="s">
-        <v>237</v>
-      </c>
-      <c r="C134" t="s">
-        <v>310</v>
-      </c>
-      <c r="D134" t="s">
-        <v>392</v>
-      </c>
-      <c r="E134" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B135" t="s">
-        <v>237</v>
-      </c>
-      <c r="C135" t="s">
-        <v>311</v>
-      </c>
-      <c r="D135" t="s">
-        <v>393</v>
-      </c>
-      <c r="E135" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B136" t="s">
-        <v>237</v>
-      </c>
-      <c r="C136" t="s">
-        <v>312</v>
-      </c>
-      <c r="D136" t="s">
-        <v>394</v>
-      </c>
-      <c r="E136" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B137" t="s">
-        <v>237</v>
-      </c>
-      <c r="C137" t="s">
-        <v>313</v>
-      </c>
-      <c r="D137" t="s">
-        <v>395</v>
-      </c>
-      <c r="E137" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B138" t="s">
-        <v>237</v>
-      </c>
-      <c r="C138" t="s">
-        <v>314</v>
-      </c>
-      <c r="D138" t="s">
-        <v>406</v>
-      </c>
-      <c r="E138" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B139" t="s">
-        <v>237</v>
-      </c>
-      <c r="C139" t="s">
-        <v>315</v>
-      </c>
-      <c r="D139" t="s">
-        <v>396</v>
-      </c>
-      <c r="E139" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B140" t="s">
-        <v>237</v>
-      </c>
-      <c r="C140" t="s">
-        <v>316</v>
-      </c>
-      <c r="D140" t="s">
-        <v>397</v>
-      </c>
-      <c r="E140" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B141" t="s">
-        <v>237</v>
-      </c>
-      <c r="C141" t="s">
-        <v>317</v>
-      </c>
-      <c r="D141" t="s">
-        <v>398</v>
-      </c>
-      <c r="E141" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B142" t="s">
-        <v>237</v>
-      </c>
-      <c r="C142" t="s">
-        <v>318</v>
-      </c>
-      <c r="D142" t="s">
-        <v>399</v>
-      </c>
-      <c r="E142" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B143" t="s">
-        <v>237</v>
-      </c>
-      <c r="C143" t="s">
-        <v>319</v>
-      </c>
-      <c r="D143" t="s">
-        <v>400</v>
-      </c>
-      <c r="E143" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B144" t="s">
-        <v>237</v>
-      </c>
-      <c r="C144" t="s">
-        <v>320</v>
-      </c>
-      <c r="D144" t="s">
-        <v>401</v>
-      </c>
-      <c r="E144" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B145" t="s">
-        <v>237</v>
-      </c>
-      <c r="C145" t="s">
-        <v>321</v>
-      </c>
-      <c r="D145" t="s">
-        <v>402</v>
-      </c>
-      <c r="E145" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B146" t="s">
-        <v>237</v>
-      </c>
-      <c r="C146" t="s">
-        <v>322</v>
-      </c>
-      <c r="D146" t="s">
-        <v>403</v>
-      </c>
-      <c r="E146" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B147" t="s">
-        <v>237</v>
-      </c>
-      <c r="C147" t="s">
-        <v>323</v>
-      </c>
-      <c r="D147" t="s">
-        <v>404</v>
-      </c>
-      <c r="E147" t="s">
-        <v>414</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Sample Collection schema to include new fields (from TGA) and updated Data Dictionary accordingly; Added Recency as Indication for VL
</commit_message>
<xml_diff>
--- a/files_and_resources/Data Dictionary.xlsx
+++ b/files_and_resources/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubarak Abdu-Aguye\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubarak\Documents\Code\LIMS-EMR-Integration\files_and_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49DEF55-4895-4323-B660-F1872FA6E461}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425D26B9-19A8-4E2B-8E2E-E763B4632F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="392">
   <si>
     <t>ID</t>
   </si>
@@ -1172,6 +1172,42 @@
   </si>
   <si>
     <t>ARV_REGIMEN_ADULT</t>
+  </si>
+  <si>
+    <t>dateScheduledForPickup</t>
+  </si>
+  <si>
+    <t>temperatureAtPickup</t>
+  </si>
+  <si>
+    <t>samplePackagedBy</t>
+  </si>
+  <si>
+    <t>courierRiderName</t>
+  </si>
+  <si>
+    <t>courierContact</t>
+  </si>
+  <si>
+    <t>The temperature of the samples at pickup time</t>
+  </si>
+  <si>
+    <t>The name of the person who packaged the samples</t>
+  </si>
+  <si>
+    <t>The name of the 3PL rider who picked up the samples</t>
+  </si>
+  <si>
+    <t>The date the samples are scheduled to be picked up</t>
+  </si>
+  <si>
+    <t>The phone number of the 3PL rider who picked up the samples</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Recency</t>
   </si>
 </sst>
 </file>
@@ -1596,10 +1632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7068A318-C14F-4D04-B583-D7B1DF373F65}">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="C109" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,123 +1781,132 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
+      <c r="C11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -1869,11 +1914,8 @@
       <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="H12" t="s">
-        <v>38</v>
-      </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1881,16 +1923,16 @@
         <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
         <v>13</v>
@@ -1904,19 +1946,16 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
         <v>13</v>
-      </c>
-      <c r="H14" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1927,10 +1966,10 @@
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
@@ -1947,10 +1986,10 @@
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
@@ -1959,7 +1998,7 @@
         <v>13</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
@@ -1970,10 +2009,10 @@
         <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -1981,8 +2020,11 @@
       <c r="G17" t="s">
         <v>13</v>
       </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
@@ -1993,16 +2035,16 @@
         <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
@@ -2013,19 +2055,19 @@
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" t="s">
-        <v>379</v>
+        <v>13</v>
+      </c>
+      <c r="H19" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
@@ -2036,10 +2078,10 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -2056,16 +2098,19 @@
         <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
+      </c>
+      <c r="I21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -2076,16 +2121,19 @@
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
@@ -2096,16 +2144,16 @@
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
         <v>45</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
@@ -2116,16 +2164,19 @@
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>57</v>
+      </c>
+      <c r="I24" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
@@ -2136,13 +2187,13 @@
         <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
         <v>13</v>
@@ -2150,19 +2201,19 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G26" t="s">
         <v>13</v>
@@ -2170,16 +2221,16 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s">
         <v>12</v>
@@ -2190,19 +2241,19 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G28" t="s">
         <v>13</v>
@@ -2210,19 +2261,19 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="G29" t="s">
         <v>13</v>
@@ -2230,19 +2281,19 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G30" t="s">
         <v>13</v>
@@ -2253,13 +2304,13 @@
         <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
         <v>12</v>
@@ -2273,13 +2324,13 @@
         <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -2287,22 +2338,19 @@
       <c r="G32" t="s">
         <v>13</v>
       </c>
-      <c r="I32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
@@ -2311,18 +2359,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
@@ -2331,18 +2379,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>73</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -2351,159 +2399,165 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C36" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" t="s">
-        <v>43</v>
-      </c>
-      <c r="E36" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="C36" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+      <c r="G36" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C37" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" t="s">
-        <v>113</v>
-      </c>
-      <c r="F37" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+      <c r="C37" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C38" t="s">
-        <v>111</v>
-      </c>
-      <c r="D38" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" t="s">
-        <v>13</v>
-      </c>
-      <c r="I38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+      <c r="C38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C39" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" t="s">
-        <v>66</v>
-      </c>
-      <c r="E39" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" t="s">
-        <v>45</v>
-      </c>
-      <c r="G39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+      <c r="C39" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" t="s">
-        <v>69</v>
-      </c>
-      <c r="F40" t="s">
-        <v>70</v>
-      </c>
-      <c r="G40" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>115</v>
+        <v>27</v>
       </c>
       <c r="F41" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
         <v>13</v>
       </c>
-      <c r="I41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D42" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
-        <v>118</v>
+        <v>24</v>
       </c>
       <c r="F42" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
         <v>13</v>
       </c>
-      <c r="H42" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>73</v>
       </c>
@@ -2511,22 +2565,19 @@
         <v>111</v>
       </c>
       <c r="D43" t="s">
-        <v>120</v>
+        <v>46</v>
       </c>
       <c r="E43" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="F43" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>57</v>
-      </c>
-      <c r="H43" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>73</v>
       </c>
@@ -2534,25 +2585,19 @@
         <v>111</v>
       </c>
       <c r="D44" t="s">
-        <v>123</v>
+        <v>29</v>
       </c>
       <c r="E44" t="s">
-        <v>124</v>
+        <v>30</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>57</v>
-      </c>
-      <c r="H44" t="s">
-        <v>122</v>
-      </c>
-      <c r="I44" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>73</v>
       </c>
@@ -2560,22 +2605,19 @@
         <v>111</v>
       </c>
       <c r="D45" t="s">
-        <v>173</v>
+        <v>31</v>
       </c>
       <c r="E45" t="s">
-        <v>174</v>
+        <v>32</v>
       </c>
       <c r="F45" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
         <v>13</v>
       </c>
-      <c r="I45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>73</v>
       </c>
@@ -2583,22 +2625,22 @@
         <v>111</v>
       </c>
       <c r="D46" t="s">
-        <v>183</v>
+        <v>43</v>
       </c>
       <c r="E46" t="s">
-        <v>184</v>
+        <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G46" t="s">
         <v>13</v>
       </c>
-      <c r="I46" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>73</v>
       </c>
@@ -2606,22 +2648,19 @@
         <v>111</v>
       </c>
       <c r="D47" t="s">
-        <v>187</v>
+        <v>112</v>
       </c>
       <c r="E47" t="s">
-        <v>188</v>
+        <v>113</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
       </c>
-      <c r="I47" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>73</v>
       </c>
@@ -2629,10 +2668,10 @@
         <v>111</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
-        <v>193</v>
+        <v>34</v>
       </c>
       <c r="F48" t="s">
         <v>12</v>
@@ -2641,7 +2680,7 @@
         <v>13</v>
       </c>
       <c r="I48" t="s">
-        <v>189</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
@@ -2652,19 +2691,16 @@
         <v>111</v>
       </c>
       <c r="D49" t="s">
-        <v>194</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>195</v>
+        <v>114</v>
       </c>
       <c r="F49" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G49" t="s">
         <v>13</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
@@ -2675,19 +2711,16 @@
         <v>111</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="G50" t="s">
         <v>13</v>
-      </c>
-      <c r="I50" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2698,10 +2731,19 @@
         <v>111</v>
       </c>
       <c r="D51" t="s">
-        <v>205</v>
+        <v>74</v>
+      </c>
+      <c r="E51" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" t="s">
+        <v>42</v>
       </c>
       <c r="G51" t="s">
-        <v>57</v>
+        <v>13</v>
+      </c>
+      <c r="I51" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
@@ -2709,13 +2751,22 @@
         <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D52" t="s">
-        <v>206</v>
+        <v>117</v>
+      </c>
+      <c r="E52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" t="s">
+        <v>108</v>
       </c>
       <c r="G52" t="s">
-        <v>57</v>
+        <v>13</v>
+      </c>
+      <c r="H52" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2726,10 +2777,19 @@
         <v>111</v>
       </c>
       <c r="D53" t="s">
-        <v>207</v>
+        <v>120</v>
+      </c>
+      <c r="E53" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" t="s">
+        <v>45</v>
       </c>
       <c r="G53" t="s">
         <v>57</v>
+      </c>
+      <c r="H53" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
@@ -2740,10 +2800,22 @@
         <v>111</v>
       </c>
       <c r="D54" t="s">
-        <v>208</v>
+        <v>123</v>
+      </c>
+      <c r="E54" t="s">
+        <v>124</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
       </c>
       <c r="G54" t="s">
         <v>57</v>
+      </c>
+      <c r="H54" t="s">
+        <v>122</v>
+      </c>
+      <c r="I54" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
@@ -2754,16 +2826,19 @@
         <v>111</v>
       </c>
       <c r="D55" t="s">
-        <v>60</v>
+        <v>173</v>
       </c>
       <c r="E55" t="s">
-        <v>61</v>
+        <v>174</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G55" t="s">
         <v>13</v>
+      </c>
+      <c r="I55" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
@@ -2774,16 +2849,19 @@
         <v>111</v>
       </c>
       <c r="D56" t="s">
-        <v>62</v>
+        <v>183</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>184</v>
       </c>
       <c r="F56" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G56" t="s">
         <v>13</v>
+      </c>
+      <c r="I56" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
@@ -2794,16 +2872,19 @@
         <v>111</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>187</v>
       </c>
       <c r="E57" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="F57" t="s">
         <v>12</v>
       </c>
       <c r="G57" t="s">
         <v>13</v>
+      </c>
+      <c r="I57" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
@@ -2814,44 +2895,56 @@
         <v>111</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>192</v>
       </c>
       <c r="E58" t="s">
-        <v>72</v>
+        <v>193</v>
       </c>
       <c r="F58" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G58" t="s">
         <v>13</v>
+      </c>
+      <c r="I58" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C59" t="s">
+        <v>111</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>194</v>
       </c>
       <c r="E59" t="s">
-        <v>77</v>
+        <v>195</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G59" t="s">
         <v>13</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C60" t="s">
+        <v>111</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
       <c r="E60" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="F60" t="s">
         <v>12</v>
@@ -2860,95 +2953,77 @@
         <v>13</v>
       </c>
       <c r="I60" t="s">
-        <v>80</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C61" t="s">
+        <v>111</v>
       </c>
       <c r="D61" t="s">
-        <v>228</v>
-      </c>
-      <c r="E61" t="s">
-        <v>229</v>
-      </c>
-      <c r="F61" t="s">
-        <v>12</v>
+        <v>205</v>
       </c>
       <c r="G61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C62" t="s">
+        <v>111</v>
       </c>
       <c r="D62" t="s">
-        <v>230</v>
-      </c>
-      <c r="E62" t="s">
-        <v>231</v>
-      </c>
-      <c r="F62" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
       <c r="G62" t="s">
-        <v>13</v>
-      </c>
-      <c r="I62" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C63" t="s">
+        <v>111</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
-      </c>
-      <c r="E63" t="s">
-        <v>79</v>
-      </c>
-      <c r="F63" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
+        <v>111</v>
       </c>
       <c r="D64" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64" t="s">
-        <v>81</v>
-      </c>
-      <c r="F64" t="s">
-        <v>12</v>
+        <v>208</v>
       </c>
       <c r="G64" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>212</v>
+        <v>73</v>
+      </c>
+      <c r="C65" t="s">
+        <v>111</v>
       </c>
       <c r="D65" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E65" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
@@ -2959,16 +3034,19 @@
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>212</v>
+        <v>73</v>
+      </c>
+      <c r="C66" t="s">
+        <v>111</v>
       </c>
       <c r="D66" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E66" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="F66" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G66" t="s">
         <v>13</v>
@@ -2976,13 +3054,16 @@
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>212</v>
+        <v>73</v>
+      </c>
+      <c r="C67" t="s">
+        <v>111</v>
       </c>
       <c r="D67" t="s">
-        <v>232</v>
+        <v>64</v>
       </c>
       <c r="E67" t="s">
-        <v>233</v>
+        <v>65</v>
       </c>
       <c r="F67" t="s">
         <v>12</v>
@@ -2993,16 +3074,19 @@
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>212</v>
+        <v>73</v>
+      </c>
+      <c r="C68" t="s">
+        <v>111</v>
       </c>
       <c r="D68" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="E68" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G68" t="s">
         <v>13</v>
@@ -3010,36 +3094,33 @@
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>212</v>
+        <v>76</v>
       </c>
       <c r="D69" t="s">
-        <v>235</v>
+        <v>10</v>
       </c>
       <c r="E69" t="s">
-        <v>236</v>
+        <v>77</v>
       </c>
       <c r="F69" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G69" t="s">
         <v>13</v>
-      </c>
-      <c r="I69" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>212</v>
+        <v>76</v>
       </c>
       <c r="D70" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="E70" t="s">
-        <v>86</v>
+        <v>227</v>
       </c>
       <c r="F70" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G70" t="s">
         <v>13</v>
@@ -3050,16 +3131,13 @@
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>212</v>
-      </c>
-      <c r="C71" t="s">
-        <v>213</v>
+        <v>76</v>
       </c>
       <c r="D71" t="s">
-        <v>23</v>
+        <v>228</v>
       </c>
       <c r="E71" t="s">
-        <v>24</v>
+        <v>229</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
@@ -3068,61 +3146,58 @@
         <v>13</v>
       </c>
       <c r="I71" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>212</v>
-      </c>
-      <c r="C72" t="s">
-        <v>213</v>
+        <v>76</v>
       </c>
       <c r="D72" t="s">
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="E72" t="s">
-        <v>27</v>
+        <v>231</v>
       </c>
       <c r="F72" t="s">
         <v>12</v>
       </c>
       <c r="G72" t="s">
         <v>13</v>
+      </c>
+      <c r="I72" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>212</v>
-      </c>
-      <c r="C73" t="s">
-        <v>214</v>
+        <v>76</v>
       </c>
       <c r="D73" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="E73" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="F73" t="s">
         <v>12</v>
       </c>
       <c r="G73" t="s">
         <v>13</v>
+      </c>
+      <c r="I73" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>212</v>
-      </c>
-      <c r="C74" t="s">
-        <v>214</v>
+        <v>76</v>
       </c>
       <c r="D74" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E74" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="F74" t="s">
         <v>12</v>
@@ -3135,37 +3210,28 @@
       <c r="B75" t="s">
         <v>212</v>
       </c>
-      <c r="C75" t="s">
-        <v>214</v>
-      </c>
       <c r="D75" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E75" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="F75" t="s">
         <v>12</v>
       </c>
       <c r="G75" t="s">
         <v>13</v>
-      </c>
-      <c r="I75" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>212</v>
       </c>
-      <c r="C76" t="s">
-        <v>214</v>
-      </c>
       <c r="D76" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="E76" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="F76" t="s">
         <v>12</v>
@@ -3178,14 +3244,11 @@
       <c r="B77" t="s">
         <v>212</v>
       </c>
-      <c r="C77" t="s">
-        <v>214</v>
-      </c>
       <c r="D77" t="s">
-        <v>46</v>
+        <v>232</v>
       </c>
       <c r="E77" t="s">
-        <v>87</v>
+        <v>233</v>
       </c>
       <c r="F77" t="s">
         <v>12</v>
@@ -3198,14 +3261,11 @@
       <c r="B78" t="s">
         <v>212</v>
       </c>
-      <c r="C78" t="s">
-        <v>214</v>
-      </c>
       <c r="D78" t="s">
-        <v>88</v>
+        <v>234</v>
       </c>
       <c r="E78" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F78" t="s">
         <v>12</v>
@@ -3218,40 +3278,40 @@
       <c r="B79" t="s">
         <v>212</v>
       </c>
-      <c r="C79" t="s">
-        <v>214</v>
-      </c>
       <c r="D79" t="s">
-        <v>90</v>
+        <v>235</v>
       </c>
       <c r="E79" t="s">
-        <v>91</v>
+        <v>236</v>
       </c>
       <c r="F79" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G79" t="s">
         <v>13</v>
+      </c>
+      <c r="I79" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>212</v>
       </c>
-      <c r="C80" t="s">
-        <v>214</v>
-      </c>
       <c r="D80" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E80" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F80" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G80" t="s">
         <v>13</v>
+      </c>
+      <c r="I80" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.3">
@@ -3259,19 +3319,22 @@
         <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D81" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="E81" t="s">
-        <v>210</v>
+        <v>24</v>
       </c>
       <c r="F81" t="s">
         <v>12</v>
       </c>
       <c r="G81" t="s">
         <v>13</v>
+      </c>
+      <c r="I81" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
@@ -3279,16 +3342,16 @@
         <v>212</v>
       </c>
       <c r="C82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D82" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="E82" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="F82" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G82" t="s">
         <v>13</v>
@@ -3302,13 +3365,13 @@
         <v>214</v>
       </c>
       <c r="D83" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="E83" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="F83" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G83" t="s">
         <v>13</v>
@@ -3322,13 +3385,13 @@
         <v>214</v>
       </c>
       <c r="D84" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="E84" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="F84" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G84" t="s">
         <v>13</v>
@@ -3342,16 +3405,19 @@
         <v>214</v>
       </c>
       <c r="D85" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="E85" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="F85" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G85" t="s">
         <v>13</v>
+      </c>
+      <c r="I85" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.3">
@@ -3362,19 +3428,16 @@
         <v>214</v>
       </c>
       <c r="D86" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="E86" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="F86" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G86" t="s">
         <v>13</v>
-      </c>
-      <c r="I86" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -3385,13 +3448,13 @@
         <v>214</v>
       </c>
       <c r="D87" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="E87" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F87" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="G87" t="s">
         <v>13</v>
@@ -3399,13 +3462,16 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="C88" t="s">
+        <v>214</v>
       </c>
       <c r="D88" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="E88" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
@@ -3416,16 +3482,19 @@
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="C89" t="s">
+        <v>214</v>
       </c>
       <c r="D89" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E89" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="F89" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G89" t="s">
         <v>13</v>
@@ -3433,16 +3502,19 @@
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="C90" t="s">
+        <v>214</v>
       </c>
       <c r="D90" t="s">
-        <v>232</v>
+        <v>92</v>
       </c>
       <c r="E90" t="s">
-        <v>233</v>
+        <v>93</v>
       </c>
       <c r="F90" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G90" t="s">
         <v>13</v>
@@ -3450,13 +3522,16 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="C91" t="s">
+        <v>214</v>
       </c>
       <c r="D91" t="s">
-        <v>234</v>
+        <v>94</v>
       </c>
       <c r="E91" t="s">
-        <v>85</v>
+        <v>210</v>
       </c>
       <c r="F91" t="s">
         <v>12</v>
@@ -3467,16 +3542,19 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="C92" t="s">
+        <v>214</v>
       </c>
       <c r="D92" t="s">
-        <v>235</v>
+        <v>95</v>
       </c>
       <c r="E92" t="s">
-        <v>236</v>
+        <v>96</v>
       </c>
       <c r="F92" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G92" t="s">
         <v>13</v>
@@ -3484,62 +3562,59 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="C93" t="s">
+        <v>214</v>
       </c>
       <c r="D93" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E93" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="F93" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G93" t="s">
         <v>13</v>
-      </c>
-      <c r="I93" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C94" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D94" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="E94" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G94" t="s">
         <v>13</v>
-      </c>
-      <c r="I94" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C95" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D95" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="E95" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G95" t="s">
         <v>13</v>
@@ -3547,39 +3622,42 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C96" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D96" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="E96" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="F96" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G96" t="s">
         <v>13</v>
+      </c>
+      <c r="I96" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C97" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D97" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E97" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="F97" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="G97" t="s">
         <v>13</v>
@@ -3589,37 +3667,28 @@
       <c r="B98" t="s">
         <v>215</v>
       </c>
-      <c r="C98" t="s">
-        <v>217</v>
-      </c>
       <c r="D98" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E98" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="F98" t="s">
         <v>12</v>
       </c>
       <c r="G98" t="s">
         <v>13</v>
-      </c>
-      <c r="I98" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>215</v>
       </c>
-      <c r="C99" t="s">
-        <v>217</v>
-      </c>
       <c r="D99" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="E99" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="F99" t="s">
         <v>12</v>
@@ -3632,14 +3701,11 @@
       <c r="B100" t="s">
         <v>215</v>
       </c>
-      <c r="C100" t="s">
-        <v>217</v>
-      </c>
       <c r="D100" t="s">
-        <v>46</v>
+        <v>232</v>
       </c>
       <c r="E100" t="s">
-        <v>87</v>
+        <v>233</v>
       </c>
       <c r="F100" t="s">
         <v>12</v>
@@ -3652,14 +3718,11 @@
       <c r="B101" t="s">
         <v>215</v>
       </c>
-      <c r="C101" t="s">
-        <v>217</v>
-      </c>
       <c r="D101" t="s">
-        <v>88</v>
+        <v>234</v>
       </c>
       <c r="E101" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F101" t="s">
         <v>12</v>
@@ -3672,17 +3735,14 @@
       <c r="B102" t="s">
         <v>215</v>
       </c>
-      <c r="C102" t="s">
-        <v>217</v>
-      </c>
       <c r="D102" t="s">
-        <v>90</v>
+        <v>235</v>
       </c>
       <c r="E102" t="s">
-        <v>91</v>
+        <v>236</v>
       </c>
       <c r="F102" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G102" t="s">
         <v>13</v>
@@ -3692,20 +3752,20 @@
       <c r="B103" t="s">
         <v>215</v>
       </c>
-      <c r="C103" t="s">
-        <v>217</v>
-      </c>
       <c r="D103" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E103" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F103" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G103" t="s">
         <v>13</v>
+      </c>
+      <c r="I103" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
@@ -3713,13 +3773,13 @@
         <v>215</v>
       </c>
       <c r="C104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D104" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="E104" t="s">
-        <v>210</v>
+        <v>24</v>
       </c>
       <c r="F104" t="s">
         <v>12</v>
@@ -3728,7 +3788,7 @@
         <v>13</v>
       </c>
       <c r="I104" t="s">
-        <v>218</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
@@ -3736,16 +3796,16 @@
         <v>215</v>
       </c>
       <c r="C105" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D105" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
       <c r="E105" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="F105" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G105" t="s">
         <v>13</v>
@@ -3759,13 +3819,13 @@
         <v>217</v>
       </c>
       <c r="D106" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="E106" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="F106" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G106" t="s">
         <v>13</v>
@@ -3779,13 +3839,13 @@
         <v>217</v>
       </c>
       <c r="D107" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="E107" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="F107" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G107" t="s">
         <v>13</v>
@@ -3799,16 +3859,19 @@
         <v>217</v>
       </c>
       <c r="D108" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
       <c r="E108" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="F108" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="G108" t="s">
         <v>13</v>
+      </c>
+      <c r="I108" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
@@ -3819,19 +3882,16 @@
         <v>217</v>
       </c>
       <c r="D109" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="E109" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="F109" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G109" t="s">
         <v>13</v>
-      </c>
-      <c r="I109" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
@@ -3842,13 +3902,13 @@
         <v>217</v>
       </c>
       <c r="D110" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="E110" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F110" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="G110" t="s">
         <v>13</v>
@@ -3862,18 +3922,224 @@
         <v>217</v>
       </c>
       <c r="D111" t="s">
+        <v>88</v>
+      </c>
+      <c r="E111" t="s">
+        <v>89</v>
+      </c>
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>215</v>
+      </c>
+      <c r="C112" t="s">
+        <v>217</v>
+      </c>
+      <c r="D112" t="s">
+        <v>90</v>
+      </c>
+      <c r="E112" t="s">
+        <v>91</v>
+      </c>
+      <c r="F112" t="s">
+        <v>45</v>
+      </c>
+      <c r="G112" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>215</v>
+      </c>
+      <c r="C113" t="s">
+        <v>217</v>
+      </c>
+      <c r="D113" t="s">
+        <v>92</v>
+      </c>
+      <c r="E113" t="s">
+        <v>93</v>
+      </c>
+      <c r="F113" t="s">
+        <v>45</v>
+      </c>
+      <c r="G113" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>215</v>
+      </c>
+      <c r="C114" t="s">
+        <v>217</v>
+      </c>
+      <c r="D114" t="s">
+        <v>94</v>
+      </c>
+      <c r="E114" t="s">
+        <v>210</v>
+      </c>
+      <c r="F114" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" t="s">
+        <v>13</v>
+      </c>
+      <c r="I114" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>215</v>
+      </c>
+      <c r="C115" t="s">
+        <v>217</v>
+      </c>
+      <c r="D115" t="s">
+        <v>95</v>
+      </c>
+      <c r="E115" t="s">
+        <v>96</v>
+      </c>
+      <c r="F115" t="s">
+        <v>45</v>
+      </c>
+      <c r="G115" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>215</v>
+      </c>
+      <c r="C116" t="s">
+        <v>217</v>
+      </c>
+      <c r="D116" t="s">
+        <v>97</v>
+      </c>
+      <c r="E116" t="s">
+        <v>98</v>
+      </c>
+      <c r="F116" t="s">
+        <v>45</v>
+      </c>
+      <c r="G116" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>215</v>
+      </c>
+      <c r="C117" t="s">
+        <v>217</v>
+      </c>
+      <c r="D117" t="s">
+        <v>99</v>
+      </c>
+      <c r="E117" t="s">
+        <v>100</v>
+      </c>
+      <c r="F117" t="s">
+        <v>45</v>
+      </c>
+      <c r="G117" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>215</v>
+      </c>
+      <c r="C118" t="s">
+        <v>217</v>
+      </c>
+      <c r="D118" t="s">
+        <v>101</v>
+      </c>
+      <c r="E118" t="s">
+        <v>102</v>
+      </c>
+      <c r="F118" t="s">
+        <v>45</v>
+      </c>
+      <c r="G118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>215</v>
+      </c>
+      <c r="C119" t="s">
+        <v>217</v>
+      </c>
+      <c r="D119" t="s">
+        <v>103</v>
+      </c>
+      <c r="E119" t="s">
+        <v>104</v>
+      </c>
+      <c r="F119" t="s">
+        <v>42</v>
+      </c>
+      <c r="G119" t="s">
+        <v>13</v>
+      </c>
+      <c r="I119" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>215</v>
+      </c>
+      <c r="C120" t="s">
+        <v>217</v>
+      </c>
+      <c r="D120" t="s">
+        <v>106</v>
+      </c>
+      <c r="E120" t="s">
+        <v>107</v>
+      </c>
+      <c r="F120" t="s">
+        <v>108</v>
+      </c>
+      <c r="G120" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>215</v>
+      </c>
+      <c r="C121" t="s">
+        <v>217</v>
+      </c>
+      <c r="D121" t="s">
         <v>219</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E121" t="s">
         <v>220</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F121" t="s">
         <v>108</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G121" t="s">
         <v>57</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I121" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3885,10 +4151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97107629-23FF-4FFF-81A6-C8B1543F2D0F}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:B130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4137,15 +4403,15 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>75</v>
+    <row r="22" spans="2:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="C22" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>156</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -4153,10 +4419,10 @@
         <v>75</v>
       </c>
       <c r="C23" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -4164,10 +4430,10 @@
         <v>75</v>
       </c>
       <c r="C24" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -4175,21 +4441,21 @@
         <v>75</v>
       </c>
       <c r="C25" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>167</v>
+        <v>75</v>
+      </c>
+      <c r="C26" s="5">
+        <v>4</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
@@ -4197,10 +4463,10 @@
         <v>166</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -4208,10 +4474,10 @@
         <v>166</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -4219,21 +4485,21 @@
         <v>166</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>175</v>
-      </c>
-      <c r="C30" s="5">
-        <v>1</v>
+        <v>166</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -4241,10 +4507,10 @@
         <v>175</v>
       </c>
       <c r="C31" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -4252,10 +4518,10 @@
         <v>175</v>
       </c>
       <c r="C32" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -4263,10 +4529,10 @@
         <v>175</v>
       </c>
       <c r="C33" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -4274,10 +4540,10 @@
         <v>175</v>
       </c>
       <c r="C34" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -4285,10 +4551,10 @@
         <v>175</v>
       </c>
       <c r="C35" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
@@ -4296,10 +4562,10 @@
         <v>175</v>
       </c>
       <c r="C36" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
@@ -4307,21 +4573,21 @@
         <v>175</v>
       </c>
       <c r="C37" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C38" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
@@ -4329,10 +4595,10 @@
         <v>185</v>
       </c>
       <c r="C39" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
@@ -4340,10 +4606,10 @@
         <v>185</v>
       </c>
       <c r="C40" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
@@ -4351,21 +4617,21 @@
         <v>185</v>
       </c>
       <c r="C41" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>189</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>200</v>
+        <v>185</v>
+      </c>
+      <c r="C42" s="5">
+        <v>4</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
@@ -4373,10 +4639,10 @@
         <v>189</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>138</v>
+        <v>200</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
@@ -4384,21 +4650,21 @@
         <v>189</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
@@ -4406,10 +4672,10 @@
         <v>199</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>202</v>
+        <v>138</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
@@ -4417,21 +4683,21 @@
         <v>199</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="5">
-        <v>1</v>
+        <v>199</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>160</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
@@ -4439,21 +4705,21 @@
         <v>80</v>
       </c>
       <c r="C49" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C50" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
@@ -4461,10 +4727,10 @@
         <v>105</v>
       </c>
       <c r="C51" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
@@ -4472,10 +4738,10 @@
         <v>105</v>
       </c>
       <c r="C52" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
@@ -4483,21 +4749,21 @@
         <v>105</v>
       </c>
       <c r="C53" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>218</v>
-      </c>
-      <c r="C54" t="s">
-        <v>167</v>
+        <v>105</v>
+      </c>
+      <c r="C54" s="5">
+        <v>4</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
@@ -4505,10 +4771,10 @@
         <v>218</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
@@ -4516,21 +4782,21 @@
         <v>218</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>221</v>
-      </c>
-      <c r="C57" s="5">
-        <v>1</v>
+        <v>218</v>
+      </c>
+      <c r="C57" t="s">
+        <v>168</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
@@ -4538,10 +4804,10 @@
         <v>221</v>
       </c>
       <c r="C58" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
@@ -4549,10 +4815,10 @@
         <v>221</v>
       </c>
       <c r="C59" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
@@ -4560,10 +4826,10 @@
         <v>221</v>
       </c>
       <c r="C60" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
@@ -4571,35 +4837,32 @@
         <v>221</v>
       </c>
       <c r="C61" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>379</v>
-      </c>
-      <c r="C62" t="s">
+        <v>221</v>
+      </c>
+      <c r="C62" s="5">
+        <v>5</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>379</v>
+      </c>
+      <c r="C63" t="s">
         <v>237</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>306</v>
-      </c>
-      <c r="E62" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="C63" t="s">
-        <v>238</v>
-      </c>
-      <c r="D63" t="s">
-        <v>307</v>
       </c>
       <c r="E63" t="s">
         <v>375</v>
@@ -4610,10 +4873,10 @@
         <v>379</v>
       </c>
       <c r="C64" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D64" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E64" t="s">
         <v>375</v>
@@ -4624,10 +4887,10 @@
         <v>379</v>
       </c>
       <c r="C65" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E65" t="s">
         <v>375</v>
@@ -4638,10 +4901,10 @@
         <v>379</v>
       </c>
       <c r="C66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E66" t="s">
         <v>375</v>
@@ -4652,10 +4915,10 @@
         <v>379</v>
       </c>
       <c r="C67" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E67" t="s">
         <v>375</v>
@@ -4666,10 +4929,10 @@
         <v>379</v>
       </c>
       <c r="C68" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D68" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E68" t="s">
         <v>375</v>
@@ -4680,10 +4943,10 @@
         <v>379</v>
       </c>
       <c r="C69" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D69" t="s">
-        <v>378</v>
+        <v>312</v>
       </c>
       <c r="E69" t="s">
         <v>375</v>
@@ -4694,10 +4957,10 @@
         <v>379</v>
       </c>
       <c r="C70" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D70" t="s">
-        <v>313</v>
+        <v>378</v>
       </c>
       <c r="E70" t="s">
         <v>375</v>
@@ -4708,10 +4971,10 @@
         <v>379</v>
       </c>
       <c r="C71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D71" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E71" t="s">
         <v>375</v>
@@ -4722,10 +4985,10 @@
         <v>379</v>
       </c>
       <c r="C72" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D72" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E72" t="s">
         <v>375</v>
@@ -4736,10 +4999,10 @@
         <v>379</v>
       </c>
       <c r="C73" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D73" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E73" t="s">
         <v>375</v>
@@ -4750,10 +5013,10 @@
         <v>379</v>
       </c>
       <c r="C74" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D74" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E74" t="s">
         <v>375</v>
@@ -4764,10 +5027,10 @@
         <v>379</v>
       </c>
       <c r="C75" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D75" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E75" t="s">
         <v>375</v>
@@ -4778,10 +5041,10 @@
         <v>379</v>
       </c>
       <c r="C76" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D76" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E76" t="s">
         <v>375</v>
@@ -4792,10 +5055,10 @@
         <v>379</v>
       </c>
       <c r="C77" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D77" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E77" t="s">
         <v>375</v>
@@ -4806,10 +5069,10 @@
         <v>379</v>
       </c>
       <c r="C78" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D78" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E78" t="s">
         <v>375</v>
@@ -4820,10 +5083,10 @@
         <v>379</v>
       </c>
       <c r="C79" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D79" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E79" t="s">
         <v>375</v>
@@ -4834,10 +5097,10 @@
         <v>379</v>
       </c>
       <c r="C80" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D80" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E80" t="s">
         <v>375</v>
@@ -4848,10 +5111,10 @@
         <v>379</v>
       </c>
       <c r="C81" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D81" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E81" t="s">
         <v>375</v>
@@ -4862,10 +5125,10 @@
         <v>379</v>
       </c>
       <c r="C82" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D82" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E82" t="s">
         <v>375</v>
@@ -4876,10 +5139,13 @@
         <v>379</v>
       </c>
       <c r="C83" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D83" t="s">
-        <v>326</v>
+        <v>325</v>
+      </c>
+      <c r="E83" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
@@ -4887,13 +5153,10 @@
         <v>379</v>
       </c>
       <c r="C84" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D84" t="s">
-        <v>327</v>
-      </c>
-      <c r="E84" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.3">
@@ -4901,10 +5164,10 @@
         <v>379</v>
       </c>
       <c r="C85" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D85" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E85" t="s">
         <v>376</v>
@@ -4915,10 +5178,10 @@
         <v>379</v>
       </c>
       <c r="C86" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D86" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E86" t="s">
         <v>376</v>
@@ -4929,10 +5192,10 @@
         <v>379</v>
       </c>
       <c r="C87" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D87" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E87" t="s">
         <v>376</v>
@@ -4943,10 +5206,10 @@
         <v>379</v>
       </c>
       <c r="C88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D88" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E88" t="s">
         <v>376</v>
@@ -4957,10 +5220,10 @@
         <v>379</v>
       </c>
       <c r="C89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D89" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E89" t="s">
         <v>376</v>
@@ -4971,10 +5234,10 @@
         <v>379</v>
       </c>
       <c r="C90" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E90" t="s">
         <v>376</v>
@@ -4985,10 +5248,10 @@
         <v>379</v>
       </c>
       <c r="C91" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D91" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E91" t="s">
         <v>376</v>
@@ -4999,10 +5262,10 @@
         <v>379</v>
       </c>
       <c r="C92" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D92" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E92" t="s">
         <v>376</v>
@@ -5013,10 +5276,10 @@
         <v>379</v>
       </c>
       <c r="C93" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D93" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E93" t="s">
         <v>376</v>
@@ -5027,10 +5290,10 @@
         <v>379</v>
       </c>
       <c r="C94" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D94" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E94" t="s">
         <v>376</v>
@@ -5041,10 +5304,10 @@
         <v>379</v>
       </c>
       <c r="C95" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E95" t="s">
         <v>376</v>
@@ -5055,10 +5318,10 @@
         <v>379</v>
       </c>
       <c r="C96" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D96" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E96" t="s">
         <v>376</v>
@@ -5069,10 +5332,10 @@
         <v>379</v>
       </c>
       <c r="C97" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D97" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E97" t="s">
         <v>376</v>
@@ -5083,10 +5346,10 @@
         <v>379</v>
       </c>
       <c r="C98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D98" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E98" t="s">
         <v>376</v>
@@ -5097,10 +5360,10 @@
         <v>379</v>
       </c>
       <c r="C99" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E99" t="s">
         <v>376</v>
@@ -5111,10 +5374,10 @@
         <v>379</v>
       </c>
       <c r="C100" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D100" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E100" t="s">
         <v>376</v>
@@ -5125,10 +5388,10 @@
         <v>379</v>
       </c>
       <c r="C101" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D101" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E101" t="s">
         <v>376</v>
@@ -5139,10 +5402,10 @@
         <v>379</v>
       </c>
       <c r="C102" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D102" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E102" t="s">
         <v>376</v>
@@ -5153,10 +5416,10 @@
         <v>379</v>
       </c>
       <c r="C103" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D103" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
       <c r="E103" t="s">
         <v>376</v>
@@ -5167,10 +5430,10 @@
         <v>379</v>
       </c>
       <c r="C104" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D104" t="s">
-        <v>346</v>
+        <v>372</v>
       </c>
       <c r="E104" t="s">
         <v>376</v>
@@ -5181,10 +5444,10 @@
         <v>379</v>
       </c>
       <c r="C105" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D105" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E105" t="s">
         <v>376</v>
@@ -5195,10 +5458,10 @@
         <v>379</v>
       </c>
       <c r="C106" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D106" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E106" t="s">
         <v>376</v>
@@ -5209,10 +5472,13 @@
         <v>379</v>
       </c>
       <c r="C107" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D107" t="s">
-        <v>349</v>
+        <v>348</v>
+      </c>
+      <c r="E107" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.3">
@@ -5220,13 +5486,10 @@
         <v>379</v>
       </c>
       <c r="C108" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D108" t="s">
-        <v>350</v>
-      </c>
-      <c r="E108" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.3">
@@ -5234,10 +5497,10 @@
         <v>379</v>
       </c>
       <c r="C109" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D109" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E109" t="s">
         <v>377</v>
@@ -5248,10 +5511,10 @@
         <v>379</v>
       </c>
       <c r="C110" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D110" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E110" t="s">
         <v>377</v>
@@ -5262,10 +5525,10 @@
         <v>379</v>
       </c>
       <c r="C111" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D111" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E111" t="s">
         <v>377</v>
@@ -5276,10 +5539,10 @@
         <v>379</v>
       </c>
       <c r="C112" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D112" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E112" t="s">
         <v>377</v>
@@ -5290,10 +5553,10 @@
         <v>379</v>
       </c>
       <c r="C113" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D113" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E113" t="s">
         <v>377</v>
@@ -5304,10 +5567,10 @@
         <v>379</v>
       </c>
       <c r="C114" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D114" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E114" t="s">
         <v>377</v>
@@ -5318,10 +5581,10 @@
         <v>379</v>
       </c>
       <c r="C115" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D115" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E115" t="s">
         <v>377</v>
@@ -5332,10 +5595,10 @@
         <v>379</v>
       </c>
       <c r="C116" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D116" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E116" t="s">
         <v>377</v>
@@ -5346,10 +5609,10 @@
         <v>379</v>
       </c>
       <c r="C117" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D117" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E117" t="s">
         <v>377</v>
@@ -5360,10 +5623,10 @@
         <v>379</v>
       </c>
       <c r="C118" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D118" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E118" t="s">
         <v>377</v>
@@ -5374,10 +5637,10 @@
         <v>379</v>
       </c>
       <c r="C119" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D119" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E119" t="s">
         <v>377</v>
@@ -5388,10 +5651,10 @@
         <v>379</v>
       </c>
       <c r="C120" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D120" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E120" t="s">
         <v>377</v>
@@ -5402,10 +5665,10 @@
         <v>379</v>
       </c>
       <c r="C121" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D121" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="E121" t="s">
         <v>377</v>
@@ -5416,10 +5679,10 @@
         <v>379</v>
       </c>
       <c r="C122" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D122" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="E122" t="s">
         <v>377</v>
@@ -5430,10 +5693,10 @@
         <v>379</v>
       </c>
       <c r="C123" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D123" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E123" t="s">
         <v>377</v>
@@ -5444,10 +5707,10 @@
         <v>379</v>
       </c>
       <c r="C124" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D124" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E124" t="s">
         <v>377</v>
@@ -5458,10 +5721,10 @@
         <v>379</v>
       </c>
       <c r="C125" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D125" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E125" t="s">
         <v>377</v>
@@ -5472,10 +5735,10 @@
         <v>379</v>
       </c>
       <c r="C126" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D126" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E126" t="s">
         <v>377</v>
@@ -5486,10 +5749,10 @@
         <v>379</v>
       </c>
       <c r="C127" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D127" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E127" t="s">
         <v>377</v>
@@ -5500,10 +5763,10 @@
         <v>379</v>
       </c>
       <c r="C128" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D128" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E128" t="s">
         <v>377</v>
@@ -5514,10 +5777,10 @@
         <v>379</v>
       </c>
       <c r="C129" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D129" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E129" t="s">
         <v>377</v>
@@ -5528,12 +5791,26 @@
         <v>379</v>
       </c>
       <c r="C130" t="s">
+        <v>304</v>
+      </c>
+      <c r="D130" t="s">
+        <v>370</v>
+      </c>
+      <c r="E130" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B131" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C131" t="s">
         <v>305</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D131" t="s">
         <v>371</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E131" t="s">
         <v>377</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data dictionary to include all regimens on NDR
</commit_message>
<xml_diff>
--- a/files_and_resources/Data Dictionary.xlsx
+++ b/files_and_resources/Data Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mubarak\Documents\Code\LIMS-EMR-Integration\files_and_resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425D26B9-19A8-4E2B-8E2E-E763B4632F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF6C06E-E69A-4A5B-AE9C-13BAC7A64363}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{24248FAC-44B2-48D7-8B29-78A82B4B6641}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="420">
   <si>
     <t>ID</t>
   </si>
@@ -1159,15 +1159,6 @@
     <t>ADDITIONAL_DESCRIPTION</t>
   </si>
   <si>
-    <t xml:space="preserve"> Adult 1st line ARV regimen </t>
-  </si>
-  <si>
-    <t>Adult 2nd line ARV regimen</t>
-  </si>
-  <si>
-    <t>Adult 3rd Line ARV Regimens</t>
-  </si>
-  <si>
     <t xml:space="preserve">TDF-3TC-AZT </t>
   </si>
   <si>
@@ -1208,6 +1199,99 @@
   </si>
   <si>
     <t>Recency</t>
+  </si>
+  <si>
+    <t>ARV_REGIMEN_CHILD</t>
+  </si>
+  <si>
+    <t>4c</t>
+  </si>
+  <si>
+    <t>ABC-3TC-EFV</t>
+  </si>
+  <si>
+    <t>4d</t>
+  </si>
+  <si>
+    <t>ABC-3TC-NVP</t>
+  </si>
+  <si>
+    <t>4f</t>
+  </si>
+  <si>
+    <t>D4T-3TC-NVP</t>
+  </si>
+  <si>
+    <t>4g</t>
+  </si>
+  <si>
+    <t>Child First Line Others</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>ABC-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>5c</t>
+  </si>
+  <si>
+    <t>D4T-3TC-LPV/r</t>
+  </si>
+  <si>
+    <t>5d</t>
+  </si>
+  <si>
+    <t>DDI-3TC-NVP</t>
+  </si>
+  <si>
+    <t>5f</t>
+  </si>
+  <si>
+    <t>Child Second Line Others</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>DRV/r + 2 NRTIs + 2 NNRTI</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t>DRV/r +2NRTIs</t>
+  </si>
+  <si>
+    <t>6c</t>
+  </si>
+  <si>
+    <t>DRV/r-DTG + 1-2 NRTIs</t>
+  </si>
+  <si>
+    <t>6d</t>
+  </si>
+  <si>
+    <t>DRV/r+RAL + 1-2NRTIs</t>
+  </si>
+  <si>
+    <t>6e</t>
+  </si>
+  <si>
+    <t>DTG+2 NRTIs</t>
+  </si>
+  <si>
+    <t>6f</t>
+  </si>
+  <si>
+    <t>RAL(or DTG) + 2 NRTIs</t>
+  </si>
+  <si>
+    <t>6g</t>
+  </si>
+  <si>
+    <t>DRV/r-2NRTIs+NNRTI</t>
   </si>
 </sst>
 </file>
@@ -1789,10 +1873,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>45</v>
@@ -1812,13 +1896,13 @@
         <v>9</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>57</v>
@@ -1835,10 +1919,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>12</v>
@@ -1858,10 +1942,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>12</v>
@@ -1881,10 +1965,10 @@
         <v>9</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>12</v>
@@ -2176,7 +2260,7 @@
         <v>57</v>
       </c>
       <c r="I24" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
@@ -2408,10 +2492,10 @@
         <v>109</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>45</v>
@@ -2431,13 +2515,13 @@
         <v>109</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>57</v>
@@ -2454,10 +2538,10 @@
         <v>109</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>12</v>
@@ -2477,10 +2561,10 @@
         <v>109</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>12</v>
@@ -2500,10 +2584,10 @@
         <v>109</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>12</v>
@@ -4151,10 +4235,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97107629-23FF-4FFF-81A6-C8B1543F2D0F}">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:D158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4411,7 +4495,7 @@
         <v>8</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -4700,7 +4784,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>80</v>
       </c>
@@ -4711,7 +4795,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>80</v>
       </c>
@@ -4722,7 +4806,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>105</v>
       </c>
@@ -4733,7 +4817,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>105</v>
       </c>
@@ -4744,7 +4828,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>105</v>
       </c>
@@ -4755,7 +4839,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>105</v>
       </c>
@@ -4766,7 +4850,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>218</v>
       </c>
@@ -4777,7 +4861,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>218</v>
       </c>
@@ -4788,7 +4872,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>218</v>
       </c>
@@ -4799,7 +4883,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>221</v>
       </c>
@@ -4810,7 +4894,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>221</v>
       </c>
@@ -4821,7 +4905,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>221</v>
       </c>
@@ -4832,7 +4916,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>221</v>
       </c>
@@ -4843,7 +4927,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>221</v>
       </c>
@@ -4854,9 +4938,9 @@
         <v>226</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C63" t="s">
         <v>237</v>
@@ -4864,13 +4948,10 @@
       <c r="D63" t="s">
         <v>306</v>
       </c>
-      <c r="E63" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C64" t="s">
         <v>238</v>
@@ -4878,13 +4959,10 @@
       <c r="D64" t="s">
         <v>307</v>
       </c>
-      <c r="E64" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C65" t="s">
         <v>239</v>
@@ -4892,13 +4970,10 @@
       <c r="D65" t="s">
         <v>308</v>
       </c>
-      <c r="E65" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C66" t="s">
         <v>240</v>
@@ -4906,13 +4981,10 @@
       <c r="D66" t="s">
         <v>309</v>
       </c>
-      <c r="E66" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C67" t="s">
         <v>241</v>
@@ -4920,13 +4992,10 @@
       <c r="D67" t="s">
         <v>310</v>
       </c>
-      <c r="E67" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C68" t="s">
         <v>242</v>
@@ -4934,13 +5003,10 @@
       <c r="D68" t="s">
         <v>311</v>
       </c>
-      <c r="E68" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C69" t="s">
         <v>243</v>
@@ -4948,27 +5014,21 @@
       <c r="D69" t="s">
         <v>312</v>
       </c>
-      <c r="E69" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C70" t="s">
         <v>244</v>
       </c>
       <c r="D70" t="s">
-        <v>378</v>
-      </c>
-      <c r="E70" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C71" t="s">
         <v>245</v>
@@ -4976,13 +5036,10 @@
       <c r="D71" t="s">
         <v>313</v>
       </c>
-      <c r="E71" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C72" t="s">
         <v>246</v>
@@ -4990,13 +5047,10 @@
       <c r="D72" t="s">
         <v>314</v>
       </c>
-      <c r="E72" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C73" t="s">
         <v>247</v>
@@ -5004,13 +5058,10 @@
       <c r="D73" t="s">
         <v>315</v>
       </c>
-      <c r="E73" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C74" t="s">
         <v>248</v>
@@ -5018,13 +5069,10 @@
       <c r="D74" t="s">
         <v>316</v>
       </c>
-      <c r="E74" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C75" t="s">
         <v>249</v>
@@ -5032,13 +5080,10 @@
       <c r="D75" t="s">
         <v>317</v>
       </c>
-      <c r="E75" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C76" t="s">
         <v>250</v>
@@ -5046,13 +5091,10 @@
       <c r="D76" t="s">
         <v>318</v>
       </c>
-      <c r="E76" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C77" t="s">
         <v>251</v>
@@ -5060,13 +5102,10 @@
       <c r="D77" t="s">
         <v>319</v>
       </c>
-      <c r="E77" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C78" t="s">
         <v>252</v>
@@ -5074,13 +5113,10 @@
       <c r="D78" t="s">
         <v>320</v>
       </c>
-      <c r="E78" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C79" t="s">
         <v>253</v>
@@ -5088,13 +5124,10 @@
       <c r="D79" t="s">
         <v>321</v>
       </c>
-      <c r="E79" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C80" t="s">
         <v>254</v>
@@ -5102,13 +5135,10 @@
       <c r="D80" t="s">
         <v>322</v>
       </c>
-      <c r="E80" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B81" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C81" t="s">
         <v>255</v>
@@ -5116,13 +5146,10 @@
       <c r="D81" t="s">
         <v>323</v>
       </c>
-      <c r="E81" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C82" t="s">
         <v>256</v>
@@ -5130,13 +5157,10 @@
       <c r="D82" t="s">
         <v>324</v>
       </c>
-      <c r="E82" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C83" t="s">
         <v>257</v>
@@ -5144,13 +5168,10 @@
       <c r="D83" t="s">
         <v>325</v>
       </c>
-      <c r="E83" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C84" t="s">
         <v>258</v>
@@ -5159,9 +5180,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C85" t="s">
         <v>259</v>
@@ -5169,13 +5190,10 @@
       <c r="D85" t="s">
         <v>327</v>
       </c>
-      <c r="E85" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C86" t="s">
         <v>260</v>
@@ -5183,13 +5201,10 @@
       <c r="D86" t="s">
         <v>328</v>
       </c>
-      <c r="E86" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C87" t="s">
         <v>261</v>
@@ -5197,13 +5212,10 @@
       <c r="D87" t="s">
         <v>329</v>
       </c>
-      <c r="E87" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C88" t="s">
         <v>262</v>
@@ -5211,13 +5223,10 @@
       <c r="D88" t="s">
         <v>330</v>
       </c>
-      <c r="E88" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C89" t="s">
         <v>263</v>
@@ -5225,13 +5234,10 @@
       <c r="D89" t="s">
         <v>331</v>
       </c>
-      <c r="E89" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B90" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C90" t="s">
         <v>264</v>
@@ -5239,13 +5245,10 @@
       <c r="D90" t="s">
         <v>332</v>
       </c>
-      <c r="E90" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B91" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C91" t="s">
         <v>265</v>
@@ -5253,13 +5256,10 @@
       <c r="D91" t="s">
         <v>333</v>
       </c>
-      <c r="E91" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B92" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C92" t="s">
         <v>266</v>
@@ -5267,13 +5267,10 @@
       <c r="D92" t="s">
         <v>334</v>
       </c>
-      <c r="E92" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C93" t="s">
         <v>267</v>
@@ -5281,13 +5278,10 @@
       <c r="D93" t="s">
         <v>335</v>
       </c>
-      <c r="E93" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C94" t="s">
         <v>268</v>
@@ -5295,13 +5289,10 @@
       <c r="D94" t="s">
         <v>336</v>
       </c>
-      <c r="E94" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C95" t="s">
         <v>269</v>
@@ -5309,13 +5300,10 @@
       <c r="D95" t="s">
         <v>337</v>
       </c>
-      <c r="E95" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B96" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C96" t="s">
         <v>270</v>
@@ -5323,13 +5311,10 @@
       <c r="D96" t="s">
         <v>338</v>
       </c>
-      <c r="E96" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C97" t="s">
         <v>271</v>
@@ -5337,13 +5322,10 @@
       <c r="D97" t="s">
         <v>339</v>
       </c>
-      <c r="E97" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C98" t="s">
         <v>272</v>
@@ -5351,13 +5333,10 @@
       <c r="D98" t="s">
         <v>340</v>
       </c>
-      <c r="E98" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C99" t="s">
         <v>273</v>
@@ -5365,13 +5344,10 @@
       <c r="D99" t="s">
         <v>341</v>
       </c>
-      <c r="E99" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C100" t="s">
         <v>274</v>
@@ -5379,13 +5355,10 @@
       <c r="D100" t="s">
         <v>342</v>
       </c>
-      <c r="E100" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C101" t="s">
         <v>275</v>
@@ -5393,13 +5366,10 @@
       <c r="D101" t="s">
         <v>343</v>
       </c>
-      <c r="E101" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C102" t="s">
         <v>276</v>
@@ -5407,13 +5377,10 @@
       <c r="D102" t="s">
         <v>344</v>
       </c>
-      <c r="E102" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C103" t="s">
         <v>277</v>
@@ -5421,13 +5388,10 @@
       <c r="D103" t="s">
         <v>345</v>
       </c>
-      <c r="E103" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C104" t="s">
         <v>278</v>
@@ -5435,13 +5399,10 @@
       <c r="D104" t="s">
         <v>372</v>
       </c>
-      <c r="E104" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C105" t="s">
         <v>279</v>
@@ -5449,13 +5410,10 @@
       <c r="D105" t="s">
         <v>346</v>
       </c>
-      <c r="E105" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C106" t="s">
         <v>280</v>
@@ -5463,13 +5421,10 @@
       <c r="D106" t="s">
         <v>347</v>
       </c>
-      <c r="E106" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C107" t="s">
         <v>281</v>
@@ -5477,13 +5432,10 @@
       <c r="D107" t="s">
         <v>348</v>
       </c>
-      <c r="E107" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C108" t="s">
         <v>282</v>
@@ -5492,9 +5444,9 @@
         <v>349</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B109" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C109" t="s">
         <v>283</v>
@@ -5502,13 +5454,10 @@
       <c r="D109" t="s">
         <v>350</v>
       </c>
-      <c r="E109" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C110" t="s">
         <v>284</v>
@@ -5516,13 +5465,10 @@
       <c r="D110" t="s">
         <v>351</v>
       </c>
-      <c r="E110" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C111" t="s">
         <v>285</v>
@@ -5530,13 +5476,10 @@
       <c r="D111" t="s">
         <v>352</v>
       </c>
-      <c r="E111" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C112" t="s">
         <v>286</v>
@@ -5544,13 +5487,10 @@
       <c r="D112" t="s">
         <v>353</v>
       </c>
-      <c r="E112" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C113" t="s">
         <v>287</v>
@@ -5558,13 +5498,10 @@
       <c r="D113" t="s">
         <v>354</v>
       </c>
-      <c r="E113" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B114" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C114" t="s">
         <v>288</v>
@@ -5572,13 +5509,10 @@
       <c r="D114" t="s">
         <v>355</v>
       </c>
-      <c r="E114" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C115" t="s">
         <v>289</v>
@@ -5586,13 +5520,10 @@
       <c r="D115" t="s">
         <v>356</v>
       </c>
-      <c r="E115" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C116" t="s">
         <v>290</v>
@@ -5600,13 +5531,10 @@
       <c r="D116" t="s">
         <v>357</v>
       </c>
-      <c r="E116" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C117" t="s">
         <v>291</v>
@@ -5614,13 +5542,10 @@
       <c r="D117" t="s">
         <v>358</v>
       </c>
-      <c r="E117" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B118" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C118" t="s">
         <v>292</v>
@@ -5628,13 +5553,10 @@
       <c r="D118" t="s">
         <v>359</v>
       </c>
-      <c r="E118" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B119" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C119" t="s">
         <v>293</v>
@@ -5642,13 +5564,10 @@
       <c r="D119" t="s">
         <v>360</v>
       </c>
-      <c r="E119" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C120" t="s">
         <v>294</v>
@@ -5656,13 +5575,10 @@
       <c r="D120" t="s">
         <v>361</v>
       </c>
-      <c r="E120" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B121" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C121" t="s">
         <v>295</v>
@@ -5670,13 +5586,10 @@
       <c r="D121" t="s">
         <v>362</v>
       </c>
-      <c r="E121" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B122" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C122" t="s">
         <v>296</v>
@@ -5684,13 +5597,10 @@
       <c r="D122" t="s">
         <v>373</v>
       </c>
-      <c r="E122" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C123" t="s">
         <v>297</v>
@@ -5698,13 +5608,10 @@
       <c r="D123" t="s">
         <v>363</v>
       </c>
-      <c r="E123" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B124" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C124" t="s">
         <v>298</v>
@@ -5712,13 +5619,10 @@
       <c r="D124" t="s">
         <v>364</v>
       </c>
-      <c r="E124" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B125" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C125" t="s">
         <v>299</v>
@@ -5726,13 +5630,10 @@
       <c r="D125" t="s">
         <v>365</v>
       </c>
-      <c r="E125" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B126" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C126" t="s">
         <v>300</v>
@@ -5740,13 +5641,10 @@
       <c r="D126" t="s">
         <v>366</v>
       </c>
-      <c r="E126" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B127" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C127" t="s">
         <v>301</v>
@@ -5754,13 +5652,10 @@
       <c r="D127" t="s">
         <v>367</v>
       </c>
-      <c r="E127" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B128" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C128" t="s">
         <v>302</v>
@@ -5768,13 +5663,10 @@
       <c r="D128" t="s">
         <v>368</v>
       </c>
-      <c r="E128" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B129" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C129" t="s">
         <v>303</v>
@@ -5782,13 +5674,10 @@
       <c r="D129" t="s">
         <v>369</v>
       </c>
-      <c r="E129" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B130" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C130" t="s">
         <v>304</v>
@@ -5796,13 +5685,10 @@
       <c r="D130" t="s">
         <v>370</v>
       </c>
-      <c r="E130" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B131" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C131" t="s">
         <v>305</v>
@@ -5810,8 +5696,302 @@
       <c r="D131" t="s">
         <v>371</v>
       </c>
-      <c r="E131" t="s">
-        <v>377</v>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>389</v>
+      </c>
+      <c r="C132" t="s">
+        <v>238</v>
+      </c>
+      <c r="D132" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>389</v>
+      </c>
+      <c r="C133" t="s">
+        <v>257</v>
+      </c>
+      <c r="D133" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>389</v>
+      </c>
+      <c r="C134" t="s">
+        <v>237</v>
+      </c>
+      <c r="D134" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>389</v>
+      </c>
+      <c r="C135" t="s">
+        <v>249</v>
+      </c>
+      <c r="D135" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>389</v>
+      </c>
+      <c r="C136" t="s">
+        <v>245</v>
+      </c>
+      <c r="D136" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>389</v>
+      </c>
+      <c r="C137" t="s">
+        <v>255</v>
+      </c>
+      <c r="D137" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>389</v>
+      </c>
+      <c r="C138" t="s">
+        <v>241</v>
+      </c>
+      <c r="D138" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>389</v>
+      </c>
+      <c r="C139" t="s">
+        <v>239</v>
+      </c>
+      <c r="D139" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>389</v>
+      </c>
+      <c r="C140" t="s">
+        <v>247</v>
+      </c>
+      <c r="D140" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>389</v>
+      </c>
+      <c r="C141" t="s">
+        <v>390</v>
+      </c>
+      <c r="D141" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>389</v>
+      </c>
+      <c r="C142" t="s">
+        <v>392</v>
+      </c>
+      <c r="D142" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>389</v>
+      </c>
+      <c r="C143" t="s">
+        <v>394</v>
+      </c>
+      <c r="D143" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>389</v>
+      </c>
+      <c r="C144" t="s">
+        <v>396</v>
+      </c>
+      <c r="D144" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>389</v>
+      </c>
+      <c r="C145" t="s">
+        <v>398</v>
+      </c>
+      <c r="D145" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>389</v>
+      </c>
+      <c r="C146" t="s">
+        <v>260</v>
+      </c>
+      <c r="D146" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>389</v>
+      </c>
+      <c r="C147" t="s">
+        <v>259</v>
+      </c>
+      <c r="D147" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>389</v>
+      </c>
+      <c r="C148" t="s">
+        <v>263</v>
+      </c>
+      <c r="D148" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>389</v>
+      </c>
+      <c r="C149" t="s">
+        <v>400</v>
+      </c>
+      <c r="D149" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>389</v>
+      </c>
+      <c r="C150" t="s">
+        <v>402</v>
+      </c>
+      <c r="D150" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>389</v>
+      </c>
+      <c r="C151" t="s">
+        <v>404</v>
+      </c>
+      <c r="D151" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
+        <v>389</v>
+      </c>
+      <c r="C152" t="s">
+        <v>406</v>
+      </c>
+      <c r="D152" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>389</v>
+      </c>
+      <c r="C153" t="s">
+        <v>408</v>
+      </c>
+      <c r="D153" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B154" t="s">
+        <v>389</v>
+      </c>
+      <c r="C154" t="s">
+        <v>410</v>
+      </c>
+      <c r="D154" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B155" t="s">
+        <v>389</v>
+      </c>
+      <c r="C155" t="s">
+        <v>412</v>
+      </c>
+      <c r="D155" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B156" t="s">
+        <v>389</v>
+      </c>
+      <c r="C156" t="s">
+        <v>414</v>
+      </c>
+      <c r="D156" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B157" t="s">
+        <v>389</v>
+      </c>
+      <c r="C157" t="s">
+        <v>416</v>
+      </c>
+      <c r="D157" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>389</v>
+      </c>
+      <c r="C158" t="s">
+        <v>418</v>
+      </c>
+      <c r="D158" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>